<commit_message>
vvc: 1. bug fix. 2. support cclm. 3. performance data update.
</commit_message>
<xml_diff>
--- a/doc/xin266vsx265.xlsx
+++ b/doc/xin266vsx265.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\encoder-perf-test\dist-2021-01-20-07-06-06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\xin26x-github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AEC077-F915-49AC-8849-2FF42F028994}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F39FD6E-1189-4962-A3A6-5869DA7EA3E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="18432" windowHeight="10020" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bd" sheetId="1" r:id="rId1"/>
@@ -61,43 +61,43 @@
     <t>8000000</t>
   </si>
   <si>
-    <t>0.37</t>
+    <t>0.4</t>
   </si>
   <si>
-    <t>-18.32</t>
+    <t>-19.37</t>
   </si>
   <si>
-    <t>0.41</t>
+    <t>0.45</t>
   </si>
   <si>
-    <t>-20.28</t>
+    <t>-21.63</t>
   </si>
   <si>
     <t>B_Kimono1_1920x1080_24</t>
   </si>
   <si>
-    <t>0.39</t>
+    <t>0.43</t>
   </si>
   <si>
-    <t>-15.0</t>
+    <t>-16.36</t>
   </si>
   <si>
-    <t>-16.19</t>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>-18.05</t>
   </si>
   <si>
     <t>B_ParkScene_1920x1080_24</t>
   </si>
   <si>
-    <t>0.4</t>
+    <t>-13.41</t>
   </si>
   <si>
-    <t>-12.61</t>
+    <t>0.49</t>
   </si>
   <si>
-    <t>0.45</t>
-  </si>
-  <si>
-    <t>-14.55</t>
+    <t>-15.82</t>
   </si>
   <si>
     <t>B_BasketballDrive_1920x1080_50</t>
@@ -106,13 +106,13 @@
     <t>0.26</t>
   </si>
   <si>
-    <t>-12.2</t>
+    <t>-12.65</t>
   </si>
   <si>
-    <t>0.33</t>
+    <t>0.35</t>
   </si>
   <si>
-    <t>-15.43</t>
+    <t>-16.46</t>
   </si>
   <si>
     <t>B_BQTerrace_1920x1080_60</t>
@@ -121,25 +121,46 @@
     <t>0.29</t>
   </si>
   <si>
-    <t>-29.32</t>
+    <t>-29.58</t>
   </si>
   <si>
-    <t>0.31</t>
+    <t>0.32</t>
   </si>
   <si>
-    <t>-30.18</t>
+    <t>-30.87</t>
   </si>
   <si>
     <t>B_Cactus_1920x1080_50</t>
   </si>
   <si>
-    <t>-22.1</t>
+    <t>0.42</t>
   </si>
   <si>
-    <t>0.43</t>
+    <t>-22.5</t>
   </si>
   <si>
-    <t>-24.29</t>
+    <t>-25.37</t>
+  </si>
+  <si>
+    <t>xin266RATE</t>
+  </si>
+  <si>
+    <t>xin266YPSNR</t>
+  </si>
+  <si>
+    <t>xin266UPSNR</t>
+  </si>
+  <si>
+    <t>xin266VPSNR</t>
+  </si>
+  <si>
+    <t>xin266YSSIM</t>
+  </si>
+  <si>
+    <t>xin266gPSNR</t>
+  </si>
+  <si>
+    <t>xin266gSSIM</t>
   </si>
   <si>
     <t>x265RATE</t>
@@ -161,27 +182,6 @@
   </si>
   <si>
     <t>x265gSSIM</t>
-  </si>
-  <si>
-    <t>xin266RATE</t>
-  </si>
-  <si>
-    <t>xin266YPSNR</t>
-  </si>
-  <si>
-    <t>xin266UPSNR</t>
-  </si>
-  <si>
-    <t>xin266VPSNR</t>
-  </si>
-  <si>
-    <t>xin266YSSIM</t>
-  </si>
-  <si>
-    <t>xin266gPSNR</t>
-  </si>
-  <si>
-    <t>xin266gSSIM</t>
   </si>
 </sst>
 </file>
@@ -341,7 +341,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4768-4746-A736-0155F59013A5}"/>
+              <c16:uniqueId val="{00000000-7218-434D-8729-43B9B427D829}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -370,19 +370,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1987.0920000000001</c:v>
+                  <c:v>1978.453</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3466.3580000000002</c:v>
+                  <c:v>3452.7660000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4953.1180000000004</c:v>
+                  <c:v>4951.6189999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6433.2489999999998</c:v>
+                  <c:v>6475.5349999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7944.2179999999998</c:v>
+                  <c:v>7971.9759999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,19 +394,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41.722000000000001</c:v>
+                  <c:v>41.764000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.941000000000003</c:v>
+                  <c:v>42.963000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.468000000000004</c:v>
+                  <c:v>43.497</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.764000000000003</c:v>
+                  <c:v>43.802999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43.99</c:v>
+                  <c:v>44.021000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,7 +414,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4768-4746-A736-0155F59013A5}"/>
+              <c16:uniqueId val="{00000001-7218-434D-8729-43B9B427D829}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -603,7 +603,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8E6B-4465-BA3A-375809242983}"/>
+              <c16:uniqueId val="{00000000-E194-4CAF-9CAA-B94AA205C79D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -632,19 +632,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1977.34</c:v>
+                  <c:v>1981.662</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3549.288</c:v>
+                  <c:v>3499.732</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5094.2889999999998</c:v>
+                  <c:v>5105.174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6771.2139999999999</c:v>
+                  <c:v>6730.768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8282.18</c:v>
+                  <c:v>8358.1919999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,7 +676,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8E6B-4465-BA3A-375809242983}"/>
+              <c16:uniqueId val="{00000001-E194-4CAF-9CAA-B94AA205C79D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -864,7 +864,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-65C0-4CB9-AF3B-D3C20B8015B5}"/>
+              <c16:uniqueId val="{00000000-6CA9-407A-B545-D79412D44DD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -893,19 +893,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1992.951</c:v>
+                  <c:v>1985.491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3480.9920000000002</c:v>
+                  <c:v>3486.3110000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4955.8090000000002</c:v>
+                  <c:v>4936.8090000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6437.7839999999997</c:v>
+                  <c:v>6475.7640000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7936.6859999999997</c:v>
+                  <c:v>7918.1149999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,19 +917,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.07</c:v>
+                  <c:v>37.106000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.143000000000001</c:v>
+                  <c:v>38.164999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.612000000000002</c:v>
+                  <c:v>38.628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.886000000000003</c:v>
+                  <c:v>38.902000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.076000000000001</c:v>
+                  <c:v>39.082999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,7 +937,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-65C0-4CB9-AF3B-D3C20B8015B5}"/>
+              <c16:uniqueId val="{00000001-6CA9-407A-B545-D79412D44DD1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1126,7 +1126,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-81D7-428B-9C8A-BDC1460246B9}"/>
+              <c16:uniqueId val="{00000000-0919-421A-9885-65AF9250FF8C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1155,19 +1155,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1992.951</c:v>
+                  <c:v>1985.491</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3480.9920000000002</c:v>
+                  <c:v>3486.3110000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4955.8090000000002</c:v>
+                  <c:v>4936.8090000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6437.7839999999997</c:v>
+                  <c:v>6475.7640000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7936.6859999999997</c:v>
+                  <c:v>7918.1149999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,10 +1182,10 @@
                   <c:v>0.91600000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.92700000000000005</c:v>
+                  <c:v>0.92800000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.93200000000000005</c:v>
+                  <c:v>0.93300000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.93500000000000005</c:v>
@@ -1199,7 +1199,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-81D7-428B-9C8A-BDC1460246B9}"/>
+              <c16:uniqueId val="{00000001-0919-421A-9885-65AF9250FF8C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1387,7 +1387,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AB3D-47CC-8198-4EB0DCAC6FB0}"/>
+              <c16:uniqueId val="{00000000-C176-4BBD-8840-316C01354B68}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1416,19 +1416,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1987.0920000000001</c:v>
+                  <c:v>1978.453</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3466.3580000000002</c:v>
+                  <c:v>3452.7660000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4953.1180000000004</c:v>
+                  <c:v>4951.6189999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6433.2489999999998</c:v>
+                  <c:v>6475.5349999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7944.2179999999998</c:v>
+                  <c:v>7971.9759999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,7 +1460,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AB3D-47CC-8198-4EB0DCAC6FB0}"/>
+              <c16:uniqueId val="{00000001-C176-4BBD-8840-316C01354B68}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1648,7 +1648,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-301A-47D2-9FA8-142B39782987}"/>
+              <c16:uniqueId val="{00000000-1521-458E-AF36-B97B5AFC6FAF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1677,19 +1677,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1711.5060000000001</c:v>
+                  <c:v>1686.3109999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3055.4520000000002</c:v>
+                  <c:v>3034.3719999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4571.2969999999996</c:v>
+                  <c:v>4586.2299999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6141.3739999999998</c:v>
+                  <c:v>6153.6540000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7682.2219999999998</c:v>
+                  <c:v>7766.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,19 +1701,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.570999999999998</c:v>
+                  <c:v>39.594000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.128999999999998</c:v>
+                  <c:v>41.17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.003999999999998</c:v>
+                  <c:v>42.031999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.512999999999998</c:v>
+                  <c:v>42.537999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.841999999999999</c:v>
+                  <c:v>42.878999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,7 +1721,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-301A-47D2-9FA8-142B39782987}"/>
+              <c16:uniqueId val="{00000001-1521-458E-AF36-B97B5AFC6FAF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1910,7 +1910,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-15AD-43B1-AE3C-EC38DFF64D39}"/>
+              <c16:uniqueId val="{00000000-DD17-4296-B32F-8FCD26A38B6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1939,19 +1939,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1711.5060000000001</c:v>
+                  <c:v>1686.3109999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3055.4520000000002</c:v>
+                  <c:v>3034.3719999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4571.2969999999996</c:v>
+                  <c:v>4586.2299999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6141.3739999999998</c:v>
+                  <c:v>6153.6540000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7682.2219999999998</c:v>
+                  <c:v>7766.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1966,16 +1966,16 @@
                   <c:v>0.94199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95399999999999996</c:v>
+                  <c:v>0.95499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.96299999999999997</c:v>
+                  <c:v>0.96399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96499999999999997</c:v>
+                  <c:v>0.96599999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1983,7 +1983,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-15AD-43B1-AE3C-EC38DFF64D39}"/>
+              <c16:uniqueId val="{00000001-DD17-4296-B32F-8FCD26A38B6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2171,7 +2171,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A042-4F4F-BB48-8414B4D084A8}"/>
+              <c16:uniqueId val="{00000000-4DFC-44DF-BF19-E12957F45A20}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2200,19 +2200,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1922.924</c:v>
+                  <c:v>1963.671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3451.047</c:v>
+                  <c:v>3399.8890000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4936.75</c:v>
+                  <c:v>4883.9679999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6447.1350000000002</c:v>
+                  <c:v>6376.2250000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7906.6490000000003</c:v>
+                  <c:v>7912.4319999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2224,19 +2224,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.860999999999997</c:v>
+                  <c:v>36.948</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.529000000000003</c:v>
+                  <c:v>38.539000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.579000000000001</c:v>
+                  <c:v>39.582000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.292000000000002</c:v>
+                  <c:v>40.304000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.807000000000002</c:v>
+                  <c:v>40.832000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,7 +2244,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A042-4F4F-BB48-8414B4D084A8}"/>
+              <c16:uniqueId val="{00000001-4DFC-44DF-BF19-E12957F45A20}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2433,7 +2433,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B898-4CFA-A85C-28B72020EBA1}"/>
+              <c16:uniqueId val="{00000000-48E2-41AA-BBD8-2C684B6007F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2462,19 +2462,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1922.924</c:v>
+                  <c:v>1963.671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3451.047</c:v>
+                  <c:v>3399.8890000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4936.75</c:v>
+                  <c:v>4883.9679999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6447.1350000000002</c:v>
+                  <c:v>6376.2250000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7906.6490000000003</c:v>
+                  <c:v>7912.4319999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2486,10 +2486,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.92200000000000004</c:v>
+                  <c:v>0.92300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94099999999999995</c:v>
+                  <c:v>0.94199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.95099999999999996</c:v>
@@ -2506,7 +2506,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B898-4CFA-A85C-28B72020EBA1}"/>
+              <c16:uniqueId val="{00000001-48E2-41AA-BBD8-2C684B6007F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2694,7 +2694,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E21E-4D8C-A590-5B5C401634AD}"/>
+              <c16:uniqueId val="{00000000-06A1-4EAF-96F7-2D335527908E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2723,19 +2723,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1998.09</c:v>
+                  <c:v>2002.9680000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3487.4630000000002</c:v>
+                  <c:v>3507.6640000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5027.4750000000004</c:v>
+                  <c:v>5002.2060000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6509.3140000000003</c:v>
+                  <c:v>6539.348</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8012.5330000000004</c:v>
+                  <c:v>8047.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2747,19 +2747,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.481999999999999</c:v>
+                  <c:v>37.512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.762</c:v>
+                  <c:v>38.795999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.417000000000002</c:v>
+                  <c:v>39.420999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.774999999999999</c:v>
+                  <c:v>39.798000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.023000000000003</c:v>
+                  <c:v>40.052999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2767,7 +2767,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E21E-4D8C-A590-5B5C401634AD}"/>
+              <c16:uniqueId val="{00000001-06A1-4EAF-96F7-2D335527908E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2956,7 +2956,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8027-476E-8345-B99AA82CD668}"/>
+              <c16:uniqueId val="{00000000-C14A-4A75-8B45-B9136ABB3658}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2985,19 +2985,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1998.09</c:v>
+                  <c:v>2002.9680000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3487.4630000000002</c:v>
+                  <c:v>3507.6640000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5027.4750000000004</c:v>
+                  <c:v>5002.2060000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6509.3140000000003</c:v>
+                  <c:v>6539.348</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8012.5330000000004</c:v>
+                  <c:v>8047.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3009,10 +3009,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
+                  <c:v>0.92100000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93300000000000005</c:v>
+                  <c:v>0.93400000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.94</c:v>
@@ -3029,7 +3029,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8027-476E-8345-B99AA82CD668}"/>
+              <c16:uniqueId val="{00000001-C14A-4A75-8B45-B9136ABB3658}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3217,7 +3217,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AE0C-4BDF-AD0C-423127603E0D}"/>
+              <c16:uniqueId val="{00000000-3ED8-416A-963D-9ED482F32D84}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3246,19 +3246,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1977.34</c:v>
+                  <c:v>1981.662</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3549.288</c:v>
+                  <c:v>3499.732</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5094.2889999999998</c:v>
+                  <c:v>5105.174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6771.2139999999999</c:v>
+                  <c:v>6730.768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8282.18</c:v>
+                  <c:v>8358.1919999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3270,16 +3270,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.249000000000002</c:v>
+                  <c:v>36.261000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.673999999999999</c:v>
+                  <c:v>36.674999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.932000000000002</c:v>
+                  <c:v>36.936</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.143999999999998</c:v>
+                  <c:v>37.142000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37.308</c:v>
@@ -3290,7 +3290,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AE0C-4BDF-AD0C-423127603E0D}"/>
+              <c16:uniqueId val="{00000001-3ED8-416A-963D-9ED482F32D84}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4187,7 +4187,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>24</v>
@@ -4204,13 +4204,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.37</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
-        <v>0.39</v>
+        <v>0.43</v>
       </c>
       <c r="D2">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="E2">
         <v>0.26</v>
@@ -4219,7 +4219,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="G2">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4227,22 +4227,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-18.32</v>
+        <v>-19.37</v>
       </c>
       <c r="C3">
-        <v>-15</v>
+        <v>-16.36</v>
       </c>
       <c r="D3">
-        <v>-12.61</v>
+        <v>-13.41</v>
       </c>
       <c r="E3">
-        <v>-12.2</v>
+        <v>-12.65</v>
       </c>
       <c r="F3">
-        <v>-29.32</v>
+        <v>-29.58</v>
       </c>
       <c r="G3">
-        <v>-22.1</v>
+        <v>-22.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4250,22 +4250,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
       <c r="C4">
-        <v>0.41</v>
+        <v>0.46</v>
       </c>
       <c r="D4">
+        <v>0.49</v>
+      </c>
+      <c r="E4">
+        <v>0.35</v>
+      </c>
+      <c r="F4">
+        <v>0.32</v>
+      </c>
+      <c r="G4">
         <v>0.45</v>
-      </c>
-      <c r="E4">
-        <v>0.33</v>
-      </c>
-      <c r="F4">
-        <v>0.31</v>
-      </c>
-      <c r="G4">
-        <v>0.43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4273,22 +4273,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-20.28</v>
+        <v>-21.63</v>
       </c>
       <c r="C5">
-        <v>-16.190000000000001</v>
+        <v>-18.05</v>
       </c>
       <c r="D5">
-        <v>-14.55</v>
+        <v>-15.82</v>
       </c>
       <c r="E5">
-        <v>-15.43</v>
+        <v>-16.46</v>
       </c>
       <c r="F5">
-        <v>-30.18</v>
+        <v>-30.87</v>
       </c>
       <c r="G5">
-        <v>-24.29</v>
+        <v>-25.37</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4340,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1947.596</v>
@@ -4372,7 +4372,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>39.904000000000003</v>
@@ -4392,7 +4392,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>43.831000000000003</v>
@@ -4412,7 +4412,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>45.2</v>
@@ -4432,7 +4432,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.94799999999999995</v>
@@ -4452,7 +4452,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>40.963999999999999</v>
@@ -4472,7 +4472,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.95599999999999996</v>
@@ -4492,87 +4492,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1987.0920000000001</v>
+        <v>1978.453</v>
       </c>
       <c r="C11">
-        <v>3466.3580000000002</v>
+        <v>3452.7660000000001</v>
       </c>
       <c r="D11">
-        <v>4953.1180000000004</v>
+        <v>4951.6189999999997</v>
       </c>
       <c r="E11">
-        <v>6433.2489999999998</v>
+        <v>6475.5349999999999</v>
       </c>
       <c r="F11">
-        <v>7944.2179999999998</v>
+        <v>7971.9759999999997</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>40.601999999999997</v>
+        <v>40.637</v>
       </c>
       <c r="C12">
-        <v>41.847999999999999</v>
+        <v>41.862000000000002</v>
       </c>
       <c r="D12">
-        <v>42.383000000000003</v>
+        <v>42.405000000000001</v>
       </c>
       <c r="E12">
-        <v>42.679000000000002</v>
+        <v>42.713000000000001</v>
       </c>
       <c r="F12">
-        <v>42.904000000000003</v>
+        <v>42.93</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>44.905000000000001</v>
+        <v>44.982999999999997</v>
       </c>
       <c r="C13">
-        <v>45.890999999999998</v>
+        <v>45.954999999999998</v>
       </c>
       <c r="D13">
-        <v>46.34</v>
+        <v>46.405999999999999</v>
       </c>
       <c r="E13">
-        <v>46.619</v>
+        <v>46.68</v>
       </c>
       <c r="F13">
-        <v>46.838000000000001</v>
+        <v>46.893000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>46.366999999999997</v>
+        <v>46.469000000000001</v>
       </c>
       <c r="C14">
-        <v>47.514000000000003</v>
+        <v>47.59</v>
       </c>
       <c r="D14">
-        <v>48.055</v>
+        <v>48.127000000000002</v>
       </c>
       <c r="E14">
-        <v>48.377000000000002</v>
+        <v>48.45</v>
       </c>
       <c r="F14">
-        <v>48.621000000000002</v>
+        <v>48.686999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.95399999999999996</v>
@@ -4584,7 +4584,7 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="E15">
-        <v>0.96699999999999997</v>
+        <v>0.96799999999999997</v>
       </c>
       <c r="F15">
         <v>0.96899999999999997</v>
@@ -4592,27 +4592,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>41.722000000000001</v>
+        <v>41.764000000000003</v>
       </c>
       <c r="C16">
-        <v>42.941000000000003</v>
+        <v>42.963000000000001</v>
       </c>
       <c r="D16">
-        <v>43.468000000000004</v>
+        <v>43.497</v>
       </c>
       <c r="E16">
-        <v>43.764000000000003</v>
+        <v>43.802999999999997</v>
       </c>
       <c r="F16">
-        <v>43.99</v>
+        <v>44.021000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.96199999999999997</v>
@@ -4674,12 +4674,12 @@
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1611.8019999999999</v>
@@ -4706,12 +4706,12 @@
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>38.012999999999998</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>40.798000000000002</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>42.066000000000003</v>
@@ -4771,7 +4771,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.93</v>
@@ -4791,7 +4791,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>38.875</v>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.93500000000000005</v>
@@ -4831,87 +4831,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1711.5060000000001</v>
+        <v>1686.3109999999999</v>
       </c>
       <c r="C11">
-        <v>3055.4520000000002</v>
+        <v>3034.3719999999998</v>
       </c>
       <c r="D11">
-        <v>4571.2969999999996</v>
+        <v>4586.2299999999996</v>
       </c>
       <c r="E11">
-        <v>6141.3739999999998</v>
+        <v>6153.6540000000005</v>
       </c>
       <c r="F11">
-        <v>7682.2219999999998</v>
+        <v>7766.51</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>38.713000000000001</v>
+        <v>38.716000000000001</v>
       </c>
       <c r="C12">
-        <v>40.369</v>
+        <v>40.395000000000003</v>
       </c>
       <c r="D12">
-        <v>41.271000000000001</v>
+        <v>41.286000000000001</v>
       </c>
       <c r="E12">
-        <v>41.776000000000003</v>
+        <v>41.793999999999997</v>
       </c>
       <c r="F12">
-        <v>42.094999999999999</v>
+        <v>42.125</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>41.527999999999999</v>
+        <v>41.689</v>
       </c>
       <c r="C13">
-        <v>42.603000000000002</v>
+        <v>42.707999999999998</v>
       </c>
       <c r="D13">
-        <v>43.273000000000003</v>
+        <v>43.351999999999997</v>
       </c>
       <c r="E13">
-        <v>43.709000000000003</v>
+        <v>43.764000000000003</v>
       </c>
       <c r="F13">
-        <v>44.015000000000001</v>
+        <v>44.08</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>42.683999999999997</v>
+        <v>42.722999999999999</v>
       </c>
       <c r="C14">
-        <v>43.945999999999998</v>
+        <v>44.033999999999999</v>
       </c>
       <c r="D14">
-        <v>44.862000000000002</v>
+        <v>44.927999999999997</v>
       </c>
       <c r="E14">
-        <v>45.51</v>
+        <v>45.563000000000002</v>
       </c>
       <c r="F14">
-        <v>45.972999999999999</v>
+        <v>46.033999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.93700000000000006</v>
@@ -4920,53 +4920,53 @@
         <v>0.95099999999999996</v>
       </c>
       <c r="D15">
-        <v>0.95699999999999996</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="E15">
-        <v>0.96</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="F15">
-        <v>0.96199999999999997</v>
+        <v>0.96299999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>39.570999999999998</v>
+        <v>39.594000000000001</v>
       </c>
       <c r="C16">
-        <v>41.128999999999998</v>
+        <v>41.17</v>
       </c>
       <c r="D16">
-        <v>42.003999999999998</v>
+        <v>42.031999999999996</v>
       </c>
       <c r="E16">
-        <v>42.512999999999998</v>
+        <v>42.537999999999997</v>
       </c>
       <c r="F16">
-        <v>42.841999999999999</v>
+        <v>42.878999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.94199999999999995</v>
       </c>
       <c r="C17">
-        <v>0.95399999999999996</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="D17">
         <v>0.96</v>
       </c>
       <c r="E17">
-        <v>0.96299999999999997</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="F17">
-        <v>0.96499999999999997</v>
+        <v>0.96599999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -5007,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
@@ -5018,7 +5018,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1834.664</v>
@@ -5050,7 +5050,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>35.253</v>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>38.774000000000001</v>
@@ -5090,7 +5090,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>39.911999999999999</v>
@@ -5110,7 +5110,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.90600000000000003</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>36.234000000000002</v>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.91</v>
@@ -5170,90 +5170,90 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1922.924</v>
+        <v>1963.671</v>
       </c>
       <c r="C11">
-        <v>3451.047</v>
+        <v>3399.8890000000001</v>
       </c>
       <c r="D11">
-        <v>4936.75</v>
+        <v>4883.9679999999998</v>
       </c>
       <c r="E11">
-        <v>6447.1350000000002</v>
+        <v>6376.2250000000004</v>
       </c>
       <c r="F11">
-        <v>7906.6490000000003</v>
+        <v>7912.4319999999998</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>35.823999999999998</v>
+        <v>35.892000000000003</v>
       </c>
       <c r="C12">
-        <v>37.588999999999999</v>
+        <v>37.581000000000003</v>
       </c>
       <c r="D12">
-        <v>38.683999999999997</v>
+        <v>38.673000000000002</v>
       </c>
       <c r="E12">
-        <v>39.420999999999999</v>
+        <v>39.421999999999997</v>
       </c>
       <c r="F12">
-        <v>39.951999999999998</v>
+        <v>39.97</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>39.759</v>
+        <v>40.030999999999999</v>
       </c>
       <c r="C13">
-        <v>40.914999999999999</v>
+        <v>41.069000000000003</v>
       </c>
       <c r="D13">
-        <v>41.692999999999998</v>
+        <v>41.804000000000002</v>
       </c>
       <c r="E13">
-        <v>42.232999999999997</v>
+        <v>42.322000000000003</v>
       </c>
       <c r="F13">
-        <v>42.613999999999997</v>
+        <v>42.688000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>40.75</v>
+        <v>40.847999999999999</v>
       </c>
       <c r="C14">
-        <v>41.945</v>
+        <v>41.970999999999997</v>
       </c>
       <c r="D14">
-        <v>42.850999999999999</v>
+        <v>42.869</v>
       </c>
       <c r="E14">
-        <v>43.555</v>
+        <v>43.57</v>
       </c>
       <c r="F14">
-        <v>44.085999999999999</v>
+        <v>44.116</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>0.91600000000000004</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="C15">
         <v>0.93899999999999995</v>
@@ -5270,33 +5270,33 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>36.860999999999997</v>
+        <v>36.948</v>
       </c>
       <c r="C16">
-        <v>38.529000000000003</v>
+        <v>38.539000000000001</v>
       </c>
       <c r="D16">
-        <v>39.579000000000001</v>
+        <v>39.582000000000001</v>
       </c>
       <c r="E16">
-        <v>40.292000000000002</v>
+        <v>40.304000000000002</v>
       </c>
       <c r="F16">
-        <v>40.807000000000002</v>
+        <v>40.832000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>0.92200000000000004</v>
+        <v>0.92300000000000004</v>
       </c>
       <c r="C17">
-        <v>0.94099999999999995</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="D17">
         <v>0.95099999999999996</v>
@@ -5357,7 +5357,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>2012.836</v>
@@ -5389,7 +5389,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>35.896000000000001</v>
@@ -5409,7 +5409,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>40.999000000000002</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>40.970999999999997</v>
@@ -5449,7 +5449,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5469,7 +5469,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>37.030999999999999</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.91300000000000003</v>
@@ -5509,87 +5509,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1998.09</v>
+        <v>2002.9680000000001</v>
       </c>
       <c r="C11">
-        <v>3487.4630000000002</v>
+        <v>3507.6640000000002</v>
       </c>
       <c r="D11">
-        <v>5027.4750000000004</v>
+        <v>5002.2060000000001</v>
       </c>
       <c r="E11">
-        <v>6509.3140000000003</v>
+        <v>6539.348</v>
       </c>
       <c r="F11">
-        <v>8012.5330000000004</v>
+        <v>8047.69</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>36.256999999999998</v>
+        <v>36.268999999999998</v>
       </c>
       <c r="C12">
-        <v>37.552999999999997</v>
+        <v>37.573</v>
       </c>
       <c r="D12">
-        <v>38.213000000000001</v>
+        <v>38.206000000000003</v>
       </c>
       <c r="E12">
-        <v>38.576000000000001</v>
+        <v>38.590000000000003</v>
       </c>
       <c r="F12">
-        <v>38.83</v>
+        <v>38.850999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>41.926000000000002</v>
+        <v>42.048999999999999</v>
       </c>
       <c r="C13">
-        <v>42.866</v>
+        <v>42.970999999999997</v>
       </c>
       <c r="D13">
-        <v>43.351999999999997</v>
+        <v>43.420999999999999</v>
       </c>
       <c r="E13">
-        <v>43.612000000000002</v>
+        <v>43.679000000000002</v>
       </c>
       <c r="F13">
-        <v>43.776000000000003</v>
+        <v>43.845999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>42.209000000000003</v>
+        <v>42.415999999999997</v>
       </c>
       <c r="C14">
-        <v>43.613</v>
+        <v>43.786000000000001</v>
       </c>
       <c r="D14">
-        <v>44.384999999999998</v>
+        <v>44.499000000000002</v>
       </c>
       <c r="E14">
-        <v>44.795000000000002</v>
+        <v>44.911999999999999</v>
       </c>
       <c r="F14">
-        <v>45.045000000000002</v>
+        <v>45.173000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5601,7 +5601,7 @@
         <v>0.92400000000000004</v>
       </c>
       <c r="E15">
-        <v>0.92800000000000005</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="F15">
         <v>0.93100000000000005</v>
@@ -5609,33 +5609,33 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>37.481999999999999</v>
+        <v>37.512</v>
       </c>
       <c r="C16">
-        <v>38.762</v>
+        <v>38.795999999999999</v>
       </c>
       <c r="D16">
-        <v>39.417000000000002</v>
+        <v>39.420999999999999</v>
       </c>
       <c r="E16">
-        <v>39.774999999999999</v>
+        <v>39.798000000000002</v>
       </c>
       <c r="F16">
-        <v>40.023000000000003</v>
+        <v>40.052999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>0.92</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="C17">
-        <v>0.93300000000000005</v>
+        <v>0.93400000000000005</v>
       </c>
       <c r="D17">
         <v>0.94</v>
@@ -5696,7 +5696,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1984.951</v>
@@ -5728,7 +5728,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>34.497</v>
@@ -5748,7 +5748,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>40.106999999999999</v>
@@ -5768,7 +5768,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>42.6</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5808,7 +5808,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>35.814999999999998</v>
@@ -5828,7 +5828,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.90900000000000003</v>
@@ -5848,87 +5848,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1977.34</v>
+        <v>1981.662</v>
       </c>
       <c r="C11">
-        <v>3549.288</v>
+        <v>3499.732</v>
       </c>
       <c r="D11">
-        <v>5094.2889999999998</v>
+        <v>5105.174</v>
       </c>
       <c r="E11">
-        <v>6771.2139999999999</v>
+        <v>6730.768</v>
       </c>
       <c r="F11">
-        <v>8282.18</v>
+        <v>8358.1919999999991</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>34.904000000000003</v>
+        <v>34.906999999999996</v>
       </c>
       <c r="C12">
-        <v>35.334000000000003</v>
+        <v>35.33</v>
       </c>
       <c r="D12">
         <v>35.591000000000001</v>
       </c>
       <c r="E12">
-        <v>35.802</v>
+        <v>35.795999999999999</v>
       </c>
       <c r="F12">
-        <v>35.968000000000004</v>
+        <v>35.965000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>40.887</v>
+        <v>40.991</v>
       </c>
       <c r="C13">
-        <v>41.286999999999999</v>
+        <v>41.338000000000001</v>
       </c>
       <c r="D13">
-        <v>41.564999999999998</v>
+        <v>41.618000000000002</v>
       </c>
       <c r="E13">
-        <v>41.793999999999997</v>
+        <v>41.835000000000001</v>
       </c>
       <c r="F13">
-        <v>41.947000000000003</v>
+        <v>41.973999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>43.15</v>
+        <v>43.228000000000002</v>
       </c>
       <c r="C14">
-        <v>43.481000000000002</v>
+        <v>43.527000000000001</v>
       </c>
       <c r="D14">
-        <v>43.732999999999997</v>
+        <v>43.765999999999998</v>
       </c>
       <c r="E14">
-        <v>43.942999999999998</v>
+        <v>43.984000000000002</v>
       </c>
       <c r="F14">
-        <v>44.1</v>
+        <v>44.122999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5940,7 +5940,7 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="E15">
-        <v>0.91200000000000003</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="F15">
         <v>0.91300000000000003</v>
@@ -5948,19 +5948,19 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>36.249000000000002</v>
+        <v>36.261000000000003</v>
       </c>
       <c r="C16">
-        <v>36.673999999999999</v>
+        <v>36.674999999999997</v>
       </c>
       <c r="D16">
-        <v>36.932000000000002</v>
+        <v>36.936</v>
       </c>
       <c r="E16">
-        <v>37.143999999999998</v>
+        <v>37.142000000000003</v>
       </c>
       <c r="F16">
         <v>37.308</v>
@@ -5968,7 +5968,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.91600000000000004</v>
@@ -6024,18 +6024,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1960.646</v>
@@ -6056,7 +6056,7 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>35.564999999999998</v>
@@ -6087,7 +6087,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>38.436</v>
@@ -6107,7 +6107,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>40.572000000000003</v>
@@ -6127,7 +6127,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.9</v>
@@ -6147,7 +6147,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>36.505000000000003</v>
@@ -6167,7 +6167,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.90700000000000003</v>
@@ -6187,87 +6187,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1992.951</v>
+        <v>1985.491</v>
       </c>
       <c r="C11">
-        <v>3480.9920000000002</v>
+        <v>3486.3110000000001</v>
       </c>
       <c r="D11">
-        <v>4955.8090000000002</v>
+        <v>4936.8090000000002</v>
       </c>
       <c r="E11">
-        <v>6437.7839999999997</v>
+        <v>6475.7640000000001</v>
       </c>
       <c r="F11">
-        <v>7936.6859999999997</v>
+        <v>7918.1149999999998</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>36.101999999999997</v>
+        <v>36.122</v>
       </c>
       <c r="C12">
-        <v>37.256999999999998</v>
+        <v>37.265999999999998</v>
       </c>
       <c r="D12">
-        <v>37.750999999999998</v>
+        <v>37.759</v>
       </c>
       <c r="E12">
-        <v>38.036999999999999</v>
+        <v>38.042999999999999</v>
       </c>
       <c r="F12">
-        <v>38.229999999999997</v>
+        <v>38.228999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>38.973999999999997</v>
+        <v>39.082000000000001</v>
       </c>
       <c r="C13">
-        <v>39.506</v>
+        <v>39.572000000000003</v>
       </c>
       <c r="D13">
-        <v>39.773000000000003</v>
+        <v>39.814</v>
       </c>
       <c r="E13">
-        <v>39.950000000000003</v>
+        <v>39.991999999999997</v>
       </c>
       <c r="F13">
-        <v>40.090000000000003</v>
+        <v>40.122</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>41.555</v>
+        <v>41.689</v>
       </c>
       <c r="C14">
-        <v>42.530999999999999</v>
+        <v>42.643999999999998</v>
       </c>
       <c r="D14">
-        <v>43.073</v>
+        <v>43.145000000000003</v>
       </c>
       <c r="E14">
-        <v>43.404000000000003</v>
+        <v>43.491999999999997</v>
       </c>
       <c r="F14">
-        <v>43.655999999999999</v>
+        <v>43.731000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.90800000000000003</v>
@@ -6287,36 +6287,36 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>37.07</v>
+        <v>37.106000000000002</v>
       </c>
       <c r="C16">
-        <v>38.143000000000001</v>
+        <v>38.164999999999999</v>
       </c>
       <c r="D16">
-        <v>38.612000000000002</v>
+        <v>38.628</v>
       </c>
       <c r="E16">
-        <v>38.886000000000003</v>
+        <v>38.902000000000001</v>
       </c>
       <c r="F16">
-        <v>39.076000000000001</v>
+        <v>39.082999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.91600000000000004</v>
       </c>
       <c r="C17">
-        <v>0.92700000000000005</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="D17">
-        <v>0.93200000000000005</v>
+        <v>0.93300000000000005</v>
       </c>
       <c r="E17">
         <v>0.93500000000000005</v>

</xml_diff>

<commit_message>
vvc:  1. bug fix.  2. make code faster.  3. decrease bdrate by 0.4%.
</commit_message>
<xml_diff>
--- a/doc/xin266vsx265.xlsx
+++ b/doc/xin266vsx265.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\xin26x-github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F39FD6E-1189-4962-A3A6-5869DA7EA3E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B926F2F4-4CE5-4E60-9D25-01F4B6BC2841}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="18432" windowHeight="10020" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bd" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="54">
   <si>
-    <t>bd_psnr{XIN266}/{X265}</t>
+    <t>bd_psnr{DEV266}/{X265}</t>
   </si>
   <si>
-    <t>bd_rate{XIN266}/{X265}</t>
+    <t>bd_rate{DEV266}/{X265}</t>
   </si>
   <si>
-    <t>bd_gpsnr{XIN266}/{X265}</t>
+    <t>bd_gpsnr{DEV266}/{X265}</t>
   </si>
   <si>
-    <t>bd_grate{XIN266}/{X265}</t>
+    <t>bd_grate{DEV266}/{X265}</t>
   </si>
   <si>
     <t>pedestrian_area</t>
@@ -64,70 +64,73 @@
     <t>0.4</t>
   </si>
   <si>
-    <t>-19.37</t>
+    <t>-19.46</t>
   </si>
   <si>
     <t>0.45</t>
   </si>
   <si>
-    <t>-21.63</t>
+    <t>-21.68</t>
   </si>
   <si>
     <t>B_Kimono1_1920x1080_24</t>
   </si>
   <si>
-    <t>0.43</t>
+    <t>0.44</t>
   </si>
   <si>
-    <t>-16.36</t>
+    <t>-16.8</t>
   </si>
   <si>
-    <t>0.46</t>
+    <t>0.47</t>
   </si>
   <si>
-    <t>-18.05</t>
+    <t>-18.4</t>
   </si>
   <si>
     <t>B_ParkScene_1920x1080_24</t>
   </si>
   <si>
-    <t>-13.41</t>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>-13.4</t>
   </si>
   <si>
     <t>0.49</t>
   </si>
   <si>
-    <t>-15.82</t>
+    <t>-15.75</t>
   </si>
   <si>
     <t>B_BasketballDrive_1920x1080_50</t>
   </si>
   <si>
-    <t>0.26</t>
+    <t>0.27</t>
   </si>
   <si>
-    <t>-12.65</t>
+    <t>-13.1</t>
   </si>
   <si>
-    <t>0.35</t>
+    <t>0.36</t>
   </si>
   <si>
-    <t>-16.46</t>
+    <t>-16.82</t>
   </si>
   <si>
     <t>B_BQTerrace_1920x1080_60</t>
   </si>
   <si>
-    <t>0.29</t>
+    <t>0.3</t>
   </si>
   <si>
-    <t>-29.58</t>
+    <t>-30.51</t>
   </si>
   <si>
     <t>0.32</t>
   </si>
   <si>
-    <t>-30.87</t>
+    <t>-31.66</t>
   </si>
   <si>
     <t>B_Cactus_1920x1080_50</t>
@@ -136,10 +139,34 @@
     <t>0.42</t>
   </si>
   <si>
-    <t>-22.5</t>
+    <t>-23.04</t>
   </si>
   <si>
-    <t>-25.37</t>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>-25.83</t>
+  </si>
+  <si>
+    <t>x265RATE</t>
+  </si>
+  <si>
+    <t>x265YPSNR</t>
+  </si>
+  <si>
+    <t>x265UPSNR</t>
+  </si>
+  <si>
+    <t>x265VPSNR</t>
+  </si>
+  <si>
+    <t>x265YSSIM</t>
+  </si>
+  <si>
+    <t>x265gPSNR</t>
+  </si>
+  <si>
+    <t>x265gSSIM</t>
   </si>
   <si>
     <t>xin266RATE</t>
@@ -161,27 +188,6 @@
   </si>
   <si>
     <t>xin266gSSIM</t>
-  </si>
-  <si>
-    <t>x265RATE</t>
-  </si>
-  <si>
-    <t>x265YPSNR</t>
-  </si>
-  <si>
-    <t>x265UPSNR</t>
-  </si>
-  <si>
-    <t>x265VPSNR</t>
-  </si>
-  <si>
-    <t>x265YSSIM</t>
-  </si>
-  <si>
-    <t>x265gPSNR</t>
-  </si>
-  <si>
-    <t>x265gSSIM</t>
   </si>
 </sst>
 </file>
@@ -341,7 +347,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7218-434D-8729-43B9B427D829}"/>
+              <c16:uniqueId val="{00000000-5BFB-4A5B-BFBB-3B8B280E89A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -370,19 +376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1978.453</c:v>
+                  <c:v>1980.788</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3452.7660000000001</c:v>
+                  <c:v>3458.9630000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4951.6189999999997</c:v>
+                  <c:v>4950.5889999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6475.5349999999999</c:v>
+                  <c:v>6435.8019999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7971.9759999999997</c:v>
+                  <c:v>7994.9960000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,19 +400,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41.764000000000003</c:v>
+                  <c:v>41.777999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.963000000000001</c:v>
+                  <c:v>42.97</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.497</c:v>
+                  <c:v>43.503999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.802999999999997</c:v>
+                  <c:v>43.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.021000000000001</c:v>
+                  <c:v>44.018999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,7 +420,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7218-434D-8729-43B9B427D829}"/>
+              <c16:uniqueId val="{00000001-5BFB-4A5B-BFBB-3B8B280E89A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -603,7 +609,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E194-4CAF-9CAA-B94AA205C79D}"/>
+              <c16:uniqueId val="{00000000-79E4-4661-830A-354DA170C8B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -632,19 +638,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1981.662</c:v>
+                  <c:v>1980.1220000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3499.732</c:v>
+                  <c:v>3479.384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5105.174</c:v>
+                  <c:v>5122.4319999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6730.768</c:v>
+                  <c:v>6738.0659999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8358.1919999999991</c:v>
+                  <c:v>8322.4959999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,7 +682,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E194-4CAF-9CAA-B94AA205C79D}"/>
+              <c16:uniqueId val="{00000001-79E4-4661-830A-354DA170C8B8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -864,7 +870,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6CA9-407A-B545-D79412D44DD1}"/>
+              <c16:uniqueId val="{00000000-F604-464D-BDF3-E5624FD587A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -893,19 +899,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1985.491</c:v>
+                  <c:v>1987.9860000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3486.3110000000001</c:v>
+                  <c:v>3478.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4936.8090000000002</c:v>
+                  <c:v>4973.3010000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6475.7640000000001</c:v>
+                  <c:v>6474.9139999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7918.1149999999998</c:v>
+                  <c:v>7915.268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,19 +923,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.106000000000002</c:v>
+                  <c:v>37.122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.164999999999999</c:v>
+                  <c:v>38.17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.628</c:v>
+                  <c:v>38.637999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.902000000000001</c:v>
+                  <c:v>38.908999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.082999999999998</c:v>
+                  <c:v>39.087000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,7 +943,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6CA9-407A-B545-D79412D44DD1}"/>
+              <c16:uniqueId val="{00000001-F604-464D-BDF3-E5624FD587A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1126,7 +1132,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0919-421A-9885-65AF9250FF8C}"/>
+              <c16:uniqueId val="{00000000-C5F4-4AB3-AC93-305BFFD7B7A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1155,19 +1161,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1985.491</c:v>
+                  <c:v>1987.9860000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3486.3110000000001</c:v>
+                  <c:v>3478.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4936.8090000000002</c:v>
+                  <c:v>4973.3010000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6475.7640000000001</c:v>
+                  <c:v>6474.9139999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7918.1149999999998</c:v>
+                  <c:v>7915.268</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1179,7 +1185,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.91600000000000004</c:v>
+                  <c:v>0.91700000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.92800000000000005</c:v>
@@ -1199,7 +1205,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0919-421A-9885-65AF9250FF8C}"/>
+              <c16:uniqueId val="{00000001-C5F4-4AB3-AC93-305BFFD7B7A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1387,7 +1393,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C176-4BBD-8840-316C01354B68}"/>
+              <c16:uniqueId val="{00000000-69CD-4171-9D67-0209A3086423}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1416,19 +1422,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1978.453</c:v>
+                  <c:v>1980.788</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3452.7660000000001</c:v>
+                  <c:v>3458.9630000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4951.6189999999997</c:v>
+                  <c:v>4950.5889999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6475.5349999999999</c:v>
+                  <c:v>6435.8019999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7971.9759999999997</c:v>
+                  <c:v>7994.9960000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,7 +1466,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C176-4BBD-8840-316C01354B68}"/>
+              <c16:uniqueId val="{00000001-69CD-4171-9D67-0209A3086423}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1648,7 +1654,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1521-458E-AF36-B97B5AFC6FAF}"/>
+              <c16:uniqueId val="{00000000-2C45-4CDD-B6D1-5D9FCB303C9C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1677,19 +1683,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1686.3109999999999</c:v>
+                  <c:v>1693.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3034.3719999999998</c:v>
+                  <c:v>3049.2339999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4586.2299999999996</c:v>
+                  <c:v>4577.2150000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6153.6540000000005</c:v>
+                  <c:v>6170.6180000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7766.51</c:v>
+                  <c:v>7775.8440000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,19 +1707,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.594000000000001</c:v>
+                  <c:v>39.625</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.17</c:v>
+                  <c:v>41.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.031999999999996</c:v>
+                  <c:v>42.036999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.537999999999997</c:v>
+                  <c:v>42.545999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.878999999999998</c:v>
+                  <c:v>42.886000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,7 +1727,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1521-458E-AF36-B97B5AFC6FAF}"/>
+              <c16:uniqueId val="{00000001-2C45-4CDD-B6D1-5D9FCB303C9C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1910,7 +1916,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DD17-4296-B32F-8FCD26A38B6B}"/>
+              <c16:uniqueId val="{00000000-E72E-4F75-AC73-9039BE5E5C81}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1939,19 +1945,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1686.3109999999999</c:v>
+                  <c:v>1693.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3034.3719999999998</c:v>
+                  <c:v>3049.2339999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4586.2299999999996</c:v>
+                  <c:v>4577.2150000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6153.6540000000005</c:v>
+                  <c:v>6170.6180000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7766.51</c:v>
+                  <c:v>7775.8440000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1983,7 +1989,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DD17-4296-B32F-8FCD26A38B6B}"/>
+              <c16:uniqueId val="{00000001-E72E-4F75-AC73-9039BE5E5C81}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2171,7 +2177,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4DFC-44DF-BF19-E12957F45A20}"/>
+              <c16:uniqueId val="{00000000-83F1-48C1-855B-59FA582E663D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2200,19 +2206,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1963.671</c:v>
+                  <c:v>1960.0609999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3399.8890000000001</c:v>
+                  <c:v>3416.0010000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4883.9679999999998</c:v>
+                  <c:v>4942.57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6376.2250000000004</c:v>
+                  <c:v>6400.5820000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7912.4319999999998</c:v>
+                  <c:v>7922.7110000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2224,19 +2230,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.948</c:v>
+                  <c:v>36.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.539000000000001</c:v>
+                  <c:v>38.551000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.582000000000001</c:v>
+                  <c:v>39.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.304000000000002</c:v>
+                  <c:v>40.311</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.832000000000001</c:v>
+                  <c:v>40.838000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,7 +2250,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4DFC-44DF-BF19-E12957F45A20}"/>
+              <c16:uniqueId val="{00000001-83F1-48C1-855B-59FA582E663D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2433,7 +2439,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-48E2-41AA-BBD8-2C684B6007F2}"/>
+              <c16:uniqueId val="{00000000-F2C3-4522-AC5B-FFA63AC82131}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2462,19 +2468,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1963.671</c:v>
+                  <c:v>1960.0609999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3399.8890000000001</c:v>
+                  <c:v>3416.0010000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4883.9679999999998</c:v>
+                  <c:v>4942.57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6376.2250000000004</c:v>
+                  <c:v>6400.5820000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7912.4319999999998</c:v>
+                  <c:v>7922.7110000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2492,7 +2498,7 @@
                   <c:v>0.94199999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95099999999999996</c:v>
+                  <c:v>0.95199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.95699999999999996</c:v>
@@ -2506,7 +2512,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-48E2-41AA-BBD8-2C684B6007F2}"/>
+              <c16:uniqueId val="{00000001-F2C3-4522-AC5B-FFA63AC82131}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2694,7 +2700,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-06A1-4EAF-96F7-2D335527908E}"/>
+              <c16:uniqueId val="{00000000-98E6-4D7C-BACC-EE408F777B14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2723,19 +2729,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2002.9680000000001</c:v>
+                  <c:v>2004.675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3507.6640000000002</c:v>
+                  <c:v>3506.422</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5002.2060000000001</c:v>
+                  <c:v>5006.317</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6539.348</c:v>
+                  <c:v>6557.3209999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8047.69</c:v>
+                  <c:v>8060.5559999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2747,19 +2753,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.512</c:v>
+                  <c:v>37.520000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.795999999999999</c:v>
+                  <c:v>38.805999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.420999999999999</c:v>
+                  <c:v>39.423999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.798000000000002</c:v>
+                  <c:v>39.801000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.052999999999997</c:v>
+                  <c:v>40.054000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2767,7 +2773,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-06A1-4EAF-96F7-2D335527908E}"/>
+              <c16:uniqueId val="{00000001-98E6-4D7C-BACC-EE408F777B14}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2956,7 +2962,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C14A-4A75-8B45-B9136ABB3658}"/>
+              <c16:uniqueId val="{00000000-FD1E-4181-8142-F1786A4B5DD8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2985,19 +2991,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2002.9680000000001</c:v>
+                  <c:v>2004.675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3507.6640000000002</c:v>
+                  <c:v>3506.422</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5002.2060000000001</c:v>
+                  <c:v>5006.317</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6539.348</c:v>
+                  <c:v>6557.3209999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8047.69</c:v>
+                  <c:v>8060.5559999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3029,7 +3035,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C14A-4A75-8B45-B9136ABB3658}"/>
+              <c16:uniqueId val="{00000001-FD1E-4181-8142-F1786A4B5DD8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3217,7 +3223,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3ED8-416A-963D-9ED482F32D84}"/>
+              <c16:uniqueId val="{00000000-C19D-4B9E-9708-57F8A12BE670}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3246,19 +3252,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1981.662</c:v>
+                  <c:v>1980.1220000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3499.732</c:v>
+                  <c:v>3479.384</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5105.174</c:v>
+                  <c:v>5122.4319999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6730.768</c:v>
+                  <c:v>6738.0659999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8358.1919999999991</c:v>
+                  <c:v>8322.4959999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3270,19 +3276,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.261000000000003</c:v>
+                  <c:v>36.264000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.674999999999997</c:v>
+                  <c:v>36.680999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.936</c:v>
+                  <c:v>36.947000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.142000000000003</c:v>
+                  <c:v>37.152000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.308</c:v>
+                  <c:v>37.311</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3290,7 +3296,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3ED8-416A-963D-9ED482F32D84}"/>
+              <c16:uniqueId val="{00000001-C19D-4B9E-9708-57F8A12BE670}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4190,13 +4196,13 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4207,16 +4213,16 @@
         <v>0.4</v>
       </c>
       <c r="C2">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="D2">
         <v>0.43</v>
       </c>
       <c r="E2">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="F2">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="G2">
         <v>0.42</v>
@@ -4227,22 +4233,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-19.37</v>
+        <v>-19.46</v>
       </c>
       <c r="C3">
-        <v>-16.36</v>
+        <v>-16.8</v>
       </c>
       <c r="D3">
-        <v>-13.41</v>
+        <v>-13.4</v>
       </c>
       <c r="E3">
-        <v>-12.65</v>
+        <v>-13.1</v>
       </c>
       <c r="F3">
-        <v>-29.58</v>
+        <v>-30.51</v>
       </c>
       <c r="G3">
-        <v>-22.5</v>
+        <v>-23.04</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4253,19 +4259,19 @@
         <v>0.45</v>
       </c>
       <c r="C4">
-        <v>0.46</v>
+        <v>0.47</v>
       </c>
       <c r="D4">
         <v>0.49</v>
       </c>
       <c r="E4">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="F4">
         <v>0.32</v>
       </c>
       <c r="G4">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4273,22 +4279,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-21.63</v>
+        <v>-21.68</v>
       </c>
       <c r="C5">
-        <v>-18.05</v>
+        <v>-18.399999999999999</v>
       </c>
       <c r="D5">
-        <v>-15.82</v>
+        <v>-15.75</v>
       </c>
       <c r="E5">
-        <v>-16.46</v>
+        <v>-16.82</v>
       </c>
       <c r="F5">
-        <v>-30.87</v>
+        <v>-31.66</v>
       </c>
       <c r="G5">
-        <v>-25.37</v>
+        <v>-25.83</v>
       </c>
     </row>
   </sheetData>
@@ -4340,7 +4346,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1947.596</v>
@@ -4372,7 +4378,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>39.904000000000003</v>
@@ -4392,7 +4398,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>43.831000000000003</v>
@@ -4412,7 +4418,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>45.2</v>
@@ -4432,7 +4438,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.94799999999999995</v>
@@ -4452,7 +4458,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>40.963999999999999</v>
@@ -4472,7 +4478,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.95599999999999996</v>
@@ -4492,87 +4498,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11">
-        <v>1978.453</v>
+        <v>1980.788</v>
       </c>
       <c r="C11">
-        <v>3452.7660000000001</v>
+        <v>3458.9630000000002</v>
       </c>
       <c r="D11">
-        <v>4951.6189999999997</v>
+        <v>4950.5889999999999</v>
       </c>
       <c r="E11">
-        <v>6475.5349999999999</v>
+        <v>6435.8019999999997</v>
       </c>
       <c r="F11">
-        <v>7971.9759999999997</v>
+        <v>7994.9960000000001</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>40.637</v>
+        <v>40.652000000000001</v>
       </c>
       <c r="C12">
-        <v>41.862000000000002</v>
+        <v>41.87</v>
       </c>
       <c r="D12">
-        <v>42.405000000000001</v>
+        <v>42.412999999999997</v>
       </c>
       <c r="E12">
-        <v>42.713000000000001</v>
+        <v>42.71</v>
       </c>
       <c r="F12">
-        <v>42.93</v>
+        <v>42.929000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>44.982999999999997</v>
+        <v>44.988</v>
       </c>
       <c r="C13">
-        <v>45.954999999999998</v>
+        <v>45.957000000000001</v>
       </c>
       <c r="D13">
         <v>46.405999999999999</v>
       </c>
       <c r="E13">
-        <v>46.68</v>
+        <v>46.677999999999997</v>
       </c>
       <c r="F13">
-        <v>46.893000000000001</v>
+        <v>46.886000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>46.469000000000001</v>
+        <v>46.484000000000002</v>
       </c>
       <c r="C14">
-        <v>47.59</v>
+        <v>47.6</v>
       </c>
       <c r="D14">
         <v>48.127000000000002</v>
       </c>
       <c r="E14">
-        <v>48.45</v>
+        <v>48.445</v>
       </c>
       <c r="F14">
-        <v>48.686999999999998</v>
+        <v>48.677999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0.95399999999999996</v>
@@ -4592,27 +4598,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16">
-        <v>41.764000000000003</v>
+        <v>41.777999999999999</v>
       </c>
       <c r="C16">
-        <v>42.963000000000001</v>
+        <v>42.97</v>
       </c>
       <c r="D16">
-        <v>43.497</v>
+        <v>43.503999999999998</v>
       </c>
       <c r="E16">
-        <v>43.802999999999997</v>
+        <v>43.8</v>
       </c>
       <c r="F16">
-        <v>44.021000000000001</v>
+        <v>44.018999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0.96199999999999997</v>
@@ -4679,7 +4685,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1611.8019999999999</v>
@@ -4711,7 +4717,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>38.012999999999998</v>
@@ -4731,7 +4737,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>40.798000000000002</v>
@@ -4751,7 +4757,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>42.066000000000003</v>
@@ -4771,7 +4777,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.93</v>
@@ -4791,7 +4797,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>38.875</v>
@@ -4811,7 +4817,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.93500000000000005</v>
@@ -4831,93 +4837,93 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11">
-        <v>1686.3109999999999</v>
+        <v>1693.04</v>
       </c>
       <c r="C11">
-        <v>3034.3719999999998</v>
+        <v>3049.2339999999999</v>
       </c>
       <c r="D11">
-        <v>4586.2299999999996</v>
+        <v>4577.2150000000001</v>
       </c>
       <c r="E11">
-        <v>6153.6540000000005</v>
+        <v>6170.6180000000004</v>
       </c>
       <c r="F11">
-        <v>7766.51</v>
+        <v>7775.8440000000001</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>38.716000000000001</v>
+        <v>38.750999999999998</v>
       </c>
       <c r="C12">
-        <v>40.395000000000003</v>
+        <v>40.418999999999997</v>
       </c>
       <c r="D12">
-        <v>41.286000000000001</v>
+        <v>41.293999999999997</v>
       </c>
       <c r="E12">
-        <v>41.793999999999997</v>
+        <v>41.802999999999997</v>
       </c>
       <c r="F12">
-        <v>42.125</v>
+        <v>42.133000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>41.689</v>
+        <v>41.704999999999998</v>
       </c>
       <c r="C13">
-        <v>42.707999999999998</v>
+        <v>42.718000000000004</v>
       </c>
       <c r="D13">
         <v>43.351999999999997</v>
       </c>
       <c r="E13">
-        <v>43.764000000000003</v>
+        <v>43.767000000000003</v>
       </c>
       <c r="F13">
-        <v>44.08</v>
+        <v>44.082000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>42.722999999999999</v>
+        <v>42.735999999999997</v>
       </c>
       <c r="C14">
-        <v>44.033999999999999</v>
+        <v>44.036999999999999</v>
       </c>
       <c r="D14">
-        <v>44.927999999999997</v>
+        <v>44.923000000000002</v>
       </c>
       <c r="E14">
-        <v>45.563000000000002</v>
+        <v>45.564</v>
       </c>
       <c r="F14">
-        <v>46.033999999999999</v>
+        <v>46.034999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0.93700000000000006</v>
       </c>
       <c r="C15">
-        <v>0.95099999999999996</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="D15">
         <v>0.95799999999999996</v>
@@ -4931,27 +4937,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16">
-        <v>39.594000000000001</v>
+        <v>39.625</v>
       </c>
       <c r="C16">
-        <v>41.17</v>
+        <v>41.19</v>
       </c>
       <c r="D16">
-        <v>42.031999999999996</v>
+        <v>42.036999999999999</v>
       </c>
       <c r="E16">
-        <v>42.537999999999997</v>
+        <v>42.545999999999999</v>
       </c>
       <c r="F16">
-        <v>42.878999999999998</v>
+        <v>42.886000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0.94199999999999995</v>
@@ -5007,18 +5013,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1834.664</v>
@@ -5039,18 +5045,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>35.253</v>
@@ -5070,7 +5076,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>38.774000000000001</v>
@@ -5090,7 +5096,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>39.911999999999999</v>
@@ -5110,7 +5116,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.90600000000000003</v>
@@ -5130,7 +5136,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>36.234000000000002</v>
@@ -5150,7 +5156,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.91</v>
@@ -5170,87 +5176,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11">
-        <v>1963.671</v>
+        <v>1960.0609999999999</v>
       </c>
       <c r="C11">
-        <v>3399.8890000000001</v>
+        <v>3416.0010000000002</v>
       </c>
       <c r="D11">
-        <v>4883.9679999999998</v>
+        <v>4942.57</v>
       </c>
       <c r="E11">
-        <v>6376.2250000000004</v>
+        <v>6400.5820000000003</v>
       </c>
       <c r="F11">
-        <v>7912.4319999999998</v>
+        <v>7922.7110000000002</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>35.892000000000003</v>
+        <v>35.887</v>
       </c>
       <c r="C12">
-        <v>37.581000000000003</v>
+        <v>37.595999999999997</v>
       </c>
       <c r="D12">
-        <v>38.673000000000002</v>
+        <v>38.703000000000003</v>
       </c>
       <c r="E12">
-        <v>39.421999999999997</v>
+        <v>39.430999999999997</v>
       </c>
       <c r="F12">
-        <v>39.97</v>
+        <v>39.976999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>40.030999999999999</v>
+        <v>40.006</v>
       </c>
       <c r="C13">
         <v>41.069000000000003</v>
       </c>
       <c r="D13">
-        <v>41.804000000000002</v>
+        <v>41.820999999999998</v>
       </c>
       <c r="E13">
-        <v>42.322000000000003</v>
+        <v>42.32</v>
       </c>
       <c r="F13">
-        <v>42.688000000000002</v>
+        <v>42.691000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>40.847999999999999</v>
+        <v>40.826999999999998</v>
       </c>
       <c r="C14">
-        <v>41.970999999999997</v>
+        <v>41.956000000000003</v>
       </c>
       <c r="D14">
-        <v>42.869</v>
+        <v>42.893999999999998</v>
       </c>
       <c r="E14">
-        <v>43.57</v>
+        <v>43.581000000000003</v>
       </c>
       <c r="F14">
-        <v>44.116</v>
+        <v>44.116999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0.91700000000000004</v>
@@ -5270,27 +5276,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16">
-        <v>36.948</v>
+        <v>36.94</v>
       </c>
       <c r="C16">
-        <v>38.539000000000001</v>
+        <v>38.551000000000002</v>
       </c>
       <c r="D16">
-        <v>39.582000000000001</v>
+        <v>39.61</v>
       </c>
       <c r="E16">
-        <v>40.304000000000002</v>
+        <v>40.311</v>
       </c>
       <c r="F16">
-        <v>40.832000000000001</v>
+        <v>40.838000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0.92300000000000004</v>
@@ -5299,7 +5305,7 @@
         <v>0.94199999999999995</v>
       </c>
       <c r="D17">
-        <v>0.95099999999999996</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="E17">
         <v>0.95699999999999996</v>
@@ -5346,18 +5352,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>2012.836</v>
@@ -5378,18 +5384,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>35.896000000000001</v>
@@ -5409,7 +5415,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>40.999000000000002</v>
@@ -5429,7 +5435,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>40.970999999999997</v>
@@ -5449,7 +5455,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5469,7 +5475,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>37.030999999999999</v>
@@ -5489,7 +5495,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.91300000000000003</v>
@@ -5509,87 +5515,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11">
-        <v>2002.9680000000001</v>
+        <v>2004.675</v>
       </c>
       <c r="C11">
-        <v>3507.6640000000002</v>
+        <v>3506.422</v>
       </c>
       <c r="D11">
-        <v>5002.2060000000001</v>
+        <v>5006.317</v>
       </c>
       <c r="E11">
-        <v>6539.348</v>
+        <v>6557.3209999999999</v>
       </c>
       <c r="F11">
-        <v>8047.69</v>
+        <v>8060.5559999999996</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>36.268999999999998</v>
+        <v>36.28</v>
       </c>
       <c r="C12">
-        <v>37.573</v>
+        <v>37.585000000000001</v>
       </c>
       <c r="D12">
-        <v>38.206000000000003</v>
+        <v>38.209000000000003</v>
       </c>
       <c r="E12">
-        <v>38.590000000000003</v>
+        <v>38.593000000000004</v>
       </c>
       <c r="F12">
-        <v>38.850999999999999</v>
+        <v>38.853000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>42.048999999999999</v>
+        <v>42.042000000000002</v>
       </c>
       <c r="C13">
-        <v>42.970999999999997</v>
+        <v>42.966999999999999</v>
       </c>
       <c r="D13">
-        <v>43.420999999999999</v>
+        <v>43.423000000000002</v>
       </c>
       <c r="E13">
-        <v>43.679000000000002</v>
+        <v>43.68</v>
       </c>
       <c r="F13">
-        <v>43.845999999999997</v>
+        <v>43.843000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>42.415999999999997</v>
+        <v>42.405999999999999</v>
       </c>
       <c r="C14">
-        <v>43.786000000000001</v>
+        <v>43.78</v>
       </c>
       <c r="D14">
-        <v>44.499000000000002</v>
+        <v>44.497</v>
       </c>
       <c r="E14">
-        <v>44.911999999999999</v>
+        <v>44.906999999999996</v>
       </c>
       <c r="F14">
-        <v>45.173000000000002</v>
+        <v>45.168999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5609,27 +5615,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16">
-        <v>37.512</v>
+        <v>37.520000000000003</v>
       </c>
       <c r="C16">
-        <v>38.795999999999999</v>
+        <v>38.805999999999997</v>
       </c>
       <c r="D16">
-        <v>39.420999999999999</v>
+        <v>39.423999999999999</v>
       </c>
       <c r="E16">
-        <v>39.798000000000002</v>
+        <v>39.801000000000002</v>
       </c>
       <c r="F16">
-        <v>40.052999999999997</v>
+        <v>40.054000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0.92100000000000004</v>
@@ -5658,7 +5664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5685,18 +5693,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1984.951</v>
@@ -5717,18 +5725,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>34.497</v>
@@ -5748,7 +5756,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>40.106999999999999</v>
@@ -5768,7 +5776,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>42.6</v>
@@ -5788,7 +5796,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5808,7 +5816,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>35.814999999999998</v>
@@ -5828,7 +5836,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.90900000000000003</v>
@@ -5848,87 +5856,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11">
-        <v>1981.662</v>
+        <v>1980.1220000000001</v>
       </c>
       <c r="C11">
-        <v>3499.732</v>
+        <v>3479.384</v>
       </c>
       <c r="D11">
-        <v>5105.174</v>
+        <v>5122.4319999999998</v>
       </c>
       <c r="E11">
-        <v>6730.768</v>
+        <v>6738.0659999999998</v>
       </c>
       <c r="F11">
-        <v>8358.1919999999991</v>
+        <v>8322.4959999999992</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>34.906999999999996</v>
+        <v>34.912999999999997</v>
       </c>
       <c r="C12">
-        <v>35.33</v>
+        <v>35.337000000000003</v>
       </c>
       <c r="D12">
-        <v>35.591000000000001</v>
+        <v>35.603999999999999</v>
       </c>
       <c r="E12">
-        <v>35.795999999999999</v>
+        <v>35.807000000000002</v>
       </c>
       <c r="F12">
-        <v>35.965000000000003</v>
+        <v>35.969000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>40.991</v>
+        <v>40.969000000000001</v>
       </c>
       <c r="C13">
-        <v>41.338000000000001</v>
+        <v>41.337000000000003</v>
       </c>
       <c r="D13">
-        <v>41.618000000000002</v>
+        <v>41.613999999999997</v>
       </c>
       <c r="E13">
-        <v>41.835000000000001</v>
+        <v>41.831000000000003</v>
       </c>
       <c r="F13">
-        <v>41.973999999999997</v>
+        <v>41.965000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>43.228000000000002</v>
+        <v>43.220999999999997</v>
       </c>
       <c r="C14">
-        <v>43.527000000000001</v>
+        <v>43.526000000000003</v>
       </c>
       <c r="D14">
-        <v>43.765999999999998</v>
+        <v>43.764000000000003</v>
       </c>
       <c r="E14">
-        <v>43.984000000000002</v>
+        <v>43.978000000000002</v>
       </c>
       <c r="F14">
-        <v>44.122999999999998</v>
+        <v>44.116999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5940,7 +5948,7 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="E15">
-        <v>0.91100000000000003</v>
+        <v>0.91200000000000003</v>
       </c>
       <c r="F15">
         <v>0.91300000000000003</v>
@@ -5948,27 +5956,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16">
-        <v>36.261000000000003</v>
+        <v>36.264000000000003</v>
       </c>
       <c r="C16">
-        <v>36.674999999999997</v>
+        <v>36.680999999999997</v>
       </c>
       <c r="D16">
-        <v>36.936</v>
+        <v>36.947000000000003</v>
       </c>
       <c r="E16">
-        <v>37.142000000000003</v>
+        <v>37.152000000000001</v>
       </c>
       <c r="F16">
-        <v>37.308</v>
+        <v>37.311</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0.91600000000000004</v>
@@ -6024,18 +6032,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1960.646</v>
@@ -6056,18 +6064,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>35.564999999999998</v>
@@ -6087,7 +6095,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>38.436</v>
@@ -6107,7 +6115,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>40.572000000000003</v>
@@ -6127,7 +6135,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>0.9</v>
@@ -6147,7 +6155,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>36.505000000000003</v>
@@ -6167,7 +6175,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>0.90700000000000003</v>
@@ -6187,87 +6195,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B11">
-        <v>1985.491</v>
+        <v>1987.9860000000001</v>
       </c>
       <c r="C11">
-        <v>3486.3110000000001</v>
+        <v>3478.125</v>
       </c>
       <c r="D11">
-        <v>4936.8090000000002</v>
+        <v>4973.3010000000004</v>
       </c>
       <c r="E11">
-        <v>6475.7640000000001</v>
+        <v>6474.9139999999998</v>
       </c>
       <c r="F11">
-        <v>7918.1149999999998</v>
+        <v>7915.268</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12">
-        <v>36.122</v>
+        <v>36.14</v>
       </c>
       <c r="C12">
-        <v>37.265999999999998</v>
+        <v>37.273000000000003</v>
       </c>
       <c r="D12">
-        <v>37.759</v>
+        <v>37.771000000000001</v>
       </c>
       <c r="E12">
-        <v>38.042999999999999</v>
+        <v>38.052</v>
       </c>
       <c r="F12">
-        <v>38.228999999999999</v>
+        <v>38.234000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>39.082000000000001</v>
+        <v>39.087000000000003</v>
       </c>
       <c r="C13">
-        <v>39.572000000000003</v>
+        <v>39.567999999999998</v>
       </c>
       <c r="D13">
-        <v>39.814</v>
+        <v>39.82</v>
       </c>
       <c r="E13">
-        <v>39.991999999999997</v>
+        <v>39.994</v>
       </c>
       <c r="F13">
-        <v>40.122</v>
+        <v>40.124000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>41.689</v>
+        <v>41.698</v>
       </c>
       <c r="C14">
-        <v>42.643999999999998</v>
+        <v>42.631999999999998</v>
       </c>
       <c r="D14">
-        <v>43.145000000000003</v>
+        <v>43.148000000000003</v>
       </c>
       <c r="E14">
-        <v>43.491999999999997</v>
+        <v>43.488</v>
       </c>
       <c r="F14">
-        <v>43.731000000000002</v>
+        <v>43.722999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B15">
         <v>0.90800000000000003</v>
@@ -6287,30 +6295,30 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B16">
-        <v>37.106000000000002</v>
+        <v>37.122</v>
       </c>
       <c r="C16">
-        <v>38.164999999999999</v>
+        <v>38.17</v>
       </c>
       <c r="D16">
-        <v>38.628</v>
+        <v>38.637999999999998</v>
       </c>
       <c r="E16">
-        <v>38.902000000000001</v>
+        <v>38.908999999999999</v>
       </c>
       <c r="F16">
-        <v>39.082999999999998</v>
+        <v>39.087000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17">
-        <v>0.91600000000000004</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="C17">
         <v>0.92800000000000005</v>

</xml_diff>

<commit_message>
update xin266 vs x265 perfor
</commit_message>
<xml_diff>
--- a/doc/xin266vsx265.xlsx
+++ b/doc/xin266vsx265.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\xin26x-github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B926F2F4-4CE5-4E60-9D25-01F4B6BC2841}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47E87F2-4BBD-4E77-90ED-21C504CF1C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bd" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
   <si>
-    <t>bd_psnr{DEV266}/{X265}</t>
+    <t>bd_psnr{XIN266}/{X265}</t>
   </si>
   <si>
-    <t>bd_rate{DEV266}/{X265}</t>
+    <t>bd_rate{XIN266}/{X265}</t>
   </si>
   <si>
-    <t>bd_gpsnr{DEV266}/{X265}</t>
+    <t>bd_gpsnr{XIN266}/{X265}</t>
   </si>
   <si>
-    <t>bd_grate{DEV266}/{X265}</t>
+    <t>bd_grate{XIN266}/{X265}</t>
   </si>
   <si>
     <t>pedestrian_area</t>
@@ -61,16 +61,16 @@
     <t>8000000</t>
   </si>
   <si>
-    <t>0.4</t>
+    <t>0.41</t>
   </si>
   <si>
-    <t>-19.46</t>
+    <t>-19.84</t>
   </si>
   <si>
-    <t>0.45</t>
+    <t>0.46</t>
   </si>
   <si>
-    <t>-21.68</t>
+    <t>-22.04</t>
   </si>
   <si>
     <t>B_Kimono1_1920x1080_24</t>
@@ -79,13 +79,13 @@
     <t>0.44</t>
   </si>
   <si>
-    <t>-16.8</t>
+    <t>-16.94</t>
   </si>
   <si>
     <t>0.47</t>
   </si>
   <si>
-    <t>-18.4</t>
+    <t>-18.54</t>
   </si>
   <si>
     <t>B_ParkScene_1920x1080_24</t>
@@ -94,13 +94,13 @@
     <t>0.43</t>
   </si>
   <si>
-    <t>-13.4</t>
+    <t>-13.44</t>
   </si>
   <si>
     <t>0.49</t>
   </si>
   <si>
-    <t>-15.75</t>
+    <t>-15.77</t>
   </si>
   <si>
     <t>B_BasketballDrive_1920x1080_50</t>
@@ -109,43 +109,37 @@
     <t>0.27</t>
   </si>
   <si>
-    <t>-13.1</t>
+    <t>-13.13</t>
   </si>
   <si>
     <t>0.36</t>
   </si>
   <si>
-    <t>-16.82</t>
+    <t>-16.83</t>
   </si>
   <si>
     <t>B_BQTerrace_1920x1080_60</t>
   </si>
   <si>
-    <t>0.3</t>
+    <t>0.31</t>
   </si>
   <si>
-    <t>-30.51</t>
+    <t>-30.95</t>
   </si>
   <si>
-    <t>0.32</t>
+    <t>0.33</t>
   </si>
   <si>
-    <t>-31.66</t>
+    <t>-31.95</t>
   </si>
   <si>
     <t>B_Cactus_1920x1080_50</t>
   </si>
   <si>
-    <t>0.42</t>
+    <t>-23.07</t>
   </si>
   <si>
-    <t>-23.04</t>
-  </si>
-  <si>
-    <t>0.46</t>
-  </si>
-  <si>
-    <t>-25.83</t>
+    <t>-25.87</t>
   </si>
   <si>
     <t>x265RATE</t>
@@ -347,7 +341,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5BFB-4A5B-BFBB-3B8B280E89A4}"/>
+              <c16:uniqueId val="{00000000-FEA6-47D1-B165-01BE171BE0A9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -376,19 +370,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1980.788</c:v>
+                  <c:v>1980.2940000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3458.9630000000002</c:v>
+                  <c:v>3456.6660000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4950.5889999999999</c:v>
+                  <c:v>4952.009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6435.8019999999997</c:v>
+                  <c:v>6455.8519999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7994.9960000000001</c:v>
+                  <c:v>8009.3339999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,19 +394,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41.777999999999999</c:v>
+                  <c:v>41.779000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.97</c:v>
+                  <c:v>42.973999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.503999999999998</c:v>
+                  <c:v>43.506999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.8</c:v>
+                  <c:v>43.808999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.018999999999998</c:v>
+                  <c:v>44.033999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,7 +414,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5BFB-4A5B-BFBB-3B8B280E89A4}"/>
+              <c16:uniqueId val="{00000001-FEA6-47D1-B165-01BE171BE0A9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -609,7 +603,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-79E4-4661-830A-354DA170C8B8}"/>
+              <c16:uniqueId val="{00000000-51B5-4A1E-B10D-F0544BABC22A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -638,19 +632,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1980.1220000000001</c:v>
+                  <c:v>1979.3810000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3479.384</c:v>
+                  <c:v>3479.8580000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5122.4319999999998</c:v>
+                  <c:v>5143.9960000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6738.0659999999998</c:v>
+                  <c:v>6669.9210000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8322.4959999999992</c:v>
+                  <c:v>8318.8340000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,7 +676,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-79E4-4661-830A-354DA170C8B8}"/>
+              <c16:uniqueId val="{00000001-51B5-4A1E-B10D-F0544BABC22A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -870,7 +864,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F604-464D-BDF3-E5624FD587A4}"/>
+              <c16:uniqueId val="{00000000-124F-4612-8B04-F154111548CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -899,19 +893,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1987.9860000000001</c:v>
+                  <c:v>1986.5650000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3478.125</c:v>
+                  <c:v>3477.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4973.3010000000004</c:v>
+                  <c:v>4969.9359999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6474.9139999999998</c:v>
+                  <c:v>6474.2889999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7915.268</c:v>
+                  <c:v>7965.0370000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,19 +917,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.122</c:v>
+                  <c:v>37.124000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>38.17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.637999999999998</c:v>
+                  <c:v>38.639000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.908999999999999</c:v>
+                  <c:v>38.911000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.087000000000003</c:v>
+                  <c:v>39.094000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -943,7 +937,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F604-464D-BDF3-E5624FD587A4}"/>
+              <c16:uniqueId val="{00000001-124F-4612-8B04-F154111548CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1132,7 +1126,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C5F4-4AB3-AC93-305BFFD7B7A2}"/>
+              <c16:uniqueId val="{00000000-0B67-47E3-BDB4-2B4EE870FCA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1161,19 +1155,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1987.9860000000001</c:v>
+                  <c:v>1986.5650000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3478.125</c:v>
+                  <c:v>3477.07</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4973.3010000000004</c:v>
+                  <c:v>4969.9359999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6474.9139999999998</c:v>
+                  <c:v>6474.2889999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7915.268</c:v>
+                  <c:v>7965.0370000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1205,7 +1199,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C5F4-4AB3-AC93-305BFFD7B7A2}"/>
+              <c16:uniqueId val="{00000001-0B67-47E3-BDB4-2B4EE870FCA4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1393,7 +1387,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-69CD-4171-9D67-0209A3086423}"/>
+              <c16:uniqueId val="{00000000-F911-4AAE-91B3-7D342C595075}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1422,19 +1416,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1980.788</c:v>
+                  <c:v>1980.2940000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3458.9630000000002</c:v>
+                  <c:v>3456.6660000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4950.5889999999999</c:v>
+                  <c:v>4952.009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6435.8019999999997</c:v>
+                  <c:v>6455.8519999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7994.9960000000001</c:v>
+                  <c:v>8009.3339999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1466,7 +1460,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-69CD-4171-9D67-0209A3086423}"/>
+              <c16:uniqueId val="{00000001-F911-4AAE-91B3-7D342C595075}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1654,7 +1648,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2C45-4CDD-B6D1-5D9FCB303C9C}"/>
+              <c16:uniqueId val="{00000000-75C7-48C8-A6BA-919745449517}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1683,19 +1677,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1693.04</c:v>
+                  <c:v>1684.6559999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3049.2339999999999</c:v>
+                  <c:v>3046.1759999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4577.2150000000001</c:v>
+                  <c:v>4593.9309999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6170.6180000000004</c:v>
+                  <c:v>6168.6819999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7775.8440000000001</c:v>
+                  <c:v>7773.2240000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1707,16 +1701,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.625</c:v>
+                  <c:v>39.616</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.19</c:v>
+                  <c:v>41.192</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.036999999999999</c:v>
+                  <c:v>42.045999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.545999999999999</c:v>
+                  <c:v>42.548000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>42.886000000000003</c:v>
@@ -1727,7 +1721,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2C45-4CDD-B6D1-5D9FCB303C9C}"/>
+              <c16:uniqueId val="{00000001-75C7-48C8-A6BA-919745449517}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1916,7 +1910,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E72E-4F75-AC73-9039BE5E5C81}"/>
+              <c16:uniqueId val="{00000000-2C15-48AC-B1D2-E0DCBF1D4B51}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1945,19 +1939,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1693.04</c:v>
+                  <c:v>1684.6559999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3049.2339999999999</c:v>
+                  <c:v>3046.1759999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4577.2150000000001</c:v>
+                  <c:v>4593.9309999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6170.6180000000004</c:v>
+                  <c:v>6168.6819999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7775.8440000000001</c:v>
+                  <c:v>7773.2240000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1989,7 +1983,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E72E-4F75-AC73-9039BE5E5C81}"/>
+              <c16:uniqueId val="{00000001-2C15-48AC-B1D2-E0DCBF1D4B51}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2177,7 +2171,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-83F1-48C1-855B-59FA582E663D}"/>
+              <c16:uniqueId val="{00000000-31B7-419A-9E7F-9D931CD07E70}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2206,19 +2200,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1960.0609999999999</c:v>
+                  <c:v>1959.002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3416.0010000000002</c:v>
+                  <c:v>3420.1909999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4942.57</c:v>
+                  <c:v>4962.3540000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6400.5820000000003</c:v>
+                  <c:v>6394.2330000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7922.7110000000002</c:v>
+                  <c:v>7935.7179999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2230,19 +2224,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.94</c:v>
+                  <c:v>36.939</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.551000000000002</c:v>
+                  <c:v>38.555</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.61</c:v>
+                  <c:v>39.621000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.311</c:v>
+                  <c:v>40.313000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.838000000000001</c:v>
+                  <c:v>40.845999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2250,7 +2244,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-83F1-48C1-855B-59FA582E663D}"/>
+              <c16:uniqueId val="{00000001-31B7-419A-9E7F-9D931CD07E70}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2439,7 +2433,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F2C3-4522-AC5B-FFA63AC82131}"/>
+              <c16:uniqueId val="{00000000-F249-42FA-B193-697FF63C25BB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2468,19 +2462,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1960.0609999999999</c:v>
+                  <c:v>1959.002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3416.0010000000002</c:v>
+                  <c:v>3420.1909999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4942.57</c:v>
+                  <c:v>4962.3540000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6400.5820000000003</c:v>
+                  <c:v>6394.2330000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7922.7110000000002</c:v>
+                  <c:v>7935.7179999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2512,7 +2506,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F2C3-4522-AC5B-FFA63AC82131}"/>
+              <c16:uniqueId val="{00000001-F249-42FA-B193-697FF63C25BB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2700,7 +2694,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-98E6-4D7C-BACC-EE408F777B14}"/>
+              <c16:uniqueId val="{00000000-571E-4F84-8C2B-1ADC36D8F9D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2729,19 +2723,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2004.675</c:v>
+                  <c:v>2005.1369999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3506.422</c:v>
+                  <c:v>3503.558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5006.317</c:v>
+                  <c:v>5004.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6557.3209999999999</c:v>
+                  <c:v>6520.0439999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8060.5559999999996</c:v>
+                  <c:v>8070.683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2753,19 +2747,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.520000000000003</c:v>
+                  <c:v>37.523000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.805999999999997</c:v>
+                  <c:v>38.805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.423999999999999</c:v>
+                  <c:v>39.426000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>39.801000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.054000000000002</c:v>
+                  <c:v>40.057000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2773,7 +2767,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-98E6-4D7C-BACC-EE408F777B14}"/>
+              <c16:uniqueId val="{00000001-571E-4F84-8C2B-1ADC36D8F9D9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2962,7 +2956,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD1E-4181-8142-F1786A4B5DD8}"/>
+              <c16:uniqueId val="{00000000-6AEC-4607-A43E-1819078A1B26}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2991,19 +2985,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2004.675</c:v>
+                  <c:v>2005.1369999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3506.422</c:v>
+                  <c:v>3503.558</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5006.317</c:v>
+                  <c:v>5004.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6557.3209999999999</c:v>
+                  <c:v>6520.0439999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8060.5559999999996</c:v>
+                  <c:v>8070.683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3035,7 +3029,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FD1E-4181-8142-F1786A4B5DD8}"/>
+              <c16:uniqueId val="{00000001-6AEC-4607-A43E-1819078A1B26}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3223,7 +3217,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C19D-4B9E-9708-57F8A12BE670}"/>
+              <c16:uniqueId val="{00000000-24C4-4E85-8822-A04F47C23AEC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3252,19 +3246,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1980.1220000000001</c:v>
+                  <c:v>1979.3810000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3479.384</c:v>
+                  <c:v>3479.8580000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5122.4319999999998</c:v>
+                  <c:v>5143.9960000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6738.0659999999998</c:v>
+                  <c:v>6669.9210000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8322.4959999999992</c:v>
+                  <c:v>8318.8340000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3276,19 +3270,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.264000000000003</c:v>
+                  <c:v>36.267000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.680999999999997</c:v>
+                  <c:v>36.683999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.947000000000003</c:v>
+                  <c:v>36.954000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.152000000000001</c:v>
+                  <c:v>37.149000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.311</c:v>
+                  <c:v>37.317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3296,7 +3290,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C19D-4B9E-9708-57F8A12BE670}"/>
+              <c16:uniqueId val="{00000001-24C4-4E85-8822-A04F47C23AEC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4181,7 +4175,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4210,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.41</v>
       </c>
       <c r="C2">
         <v>0.44</v>
@@ -4222,10 +4218,10 @@
         <v>0.27</v>
       </c>
       <c r="F2">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="G2">
-        <v>0.42</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4233,22 +4229,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-19.46</v>
+        <v>-19.84</v>
       </c>
       <c r="C3">
-        <v>-16.8</v>
+        <v>-16.940000000000001</v>
       </c>
       <c r="D3">
-        <v>-13.4</v>
+        <v>-13.44</v>
       </c>
       <c r="E3">
-        <v>-13.1</v>
+        <v>-13.13</v>
       </c>
       <c r="F3">
-        <v>-30.51</v>
+        <v>-30.95</v>
       </c>
       <c r="G3">
-        <v>-23.04</v>
+        <v>-23.07</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4256,7 +4252,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="C4">
         <v>0.47</v>
@@ -4268,7 +4264,7 @@
         <v>0.36</v>
       </c>
       <c r="F4">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
       <c r="G4">
         <v>0.46</v>
@@ -4279,22 +4275,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-21.68</v>
+        <v>-22.04</v>
       </c>
       <c r="C5">
-        <v>-18.399999999999999</v>
+        <v>-18.54</v>
       </c>
       <c r="D5">
-        <v>-15.75</v>
+        <v>-15.77</v>
       </c>
       <c r="E5">
-        <v>-16.82</v>
+        <v>-16.829999999999998</v>
       </c>
       <c r="F5">
-        <v>-31.66</v>
+        <v>-31.95</v>
       </c>
       <c r="G5">
-        <v>-25.83</v>
+        <v>-25.87</v>
       </c>
     </row>
   </sheetData>
@@ -4346,7 +4342,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1947.596</v>
@@ -4378,7 +4374,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>39.904000000000003</v>
@@ -4398,7 +4394,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>43.831000000000003</v>
@@ -4418,7 +4414,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>45.2</v>
@@ -4438,7 +4434,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.94799999999999995</v>
@@ -4458,7 +4454,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>40.963999999999999</v>
@@ -4478,7 +4474,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0.95599999999999996</v>
@@ -4498,87 +4494,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>1980.788</v>
+        <v>1980.2940000000001</v>
       </c>
       <c r="C11">
-        <v>3458.9630000000002</v>
+        <v>3456.6660000000002</v>
       </c>
       <c r="D11">
-        <v>4950.5889999999999</v>
+        <v>4952.009</v>
       </c>
       <c r="E11">
-        <v>6435.8019999999997</v>
+        <v>6455.8519999999999</v>
       </c>
       <c r="F11">
-        <v>7994.9960000000001</v>
+        <v>8009.3339999999998</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12">
-        <v>40.652000000000001</v>
+        <v>40.654000000000003</v>
       </c>
       <c r="C12">
-        <v>41.87</v>
+        <v>41.874000000000002</v>
       </c>
       <c r="D12">
-        <v>42.412999999999997</v>
+        <v>42.415999999999997</v>
       </c>
       <c r="E12">
-        <v>42.71</v>
+        <v>42.719000000000001</v>
       </c>
       <c r="F12">
-        <v>42.929000000000002</v>
+        <v>42.944000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <v>44.988</v>
+        <v>44.99</v>
       </c>
       <c r="C13">
-        <v>45.957000000000001</v>
+        <v>45.957999999999998</v>
       </c>
       <c r="D13">
-        <v>46.405999999999999</v>
+        <v>46.402999999999999</v>
       </c>
       <c r="E13">
-        <v>46.677999999999997</v>
+        <v>46.682000000000002</v>
       </c>
       <c r="F13">
-        <v>46.886000000000003</v>
+        <v>46.896999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
-        <v>46.484000000000002</v>
+        <v>46.47</v>
       </c>
       <c r="C14">
-        <v>47.6</v>
+        <v>47.603999999999999</v>
       </c>
       <c r="D14">
         <v>48.127000000000002</v>
       </c>
       <c r="E14">
-        <v>48.445</v>
+        <v>48.45</v>
       </c>
       <c r="F14">
-        <v>48.677999999999997</v>
+        <v>48.694000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>0.95399999999999996</v>
@@ -4598,27 +4594,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>41.777999999999999</v>
+        <v>41.779000000000003</v>
       </c>
       <c r="C16">
-        <v>42.97</v>
+        <v>42.973999999999997</v>
       </c>
       <c r="D16">
-        <v>43.503999999999998</v>
+        <v>43.506999999999998</v>
       </c>
       <c r="E16">
-        <v>43.8</v>
+        <v>43.808999999999997</v>
       </c>
       <c r="F16">
-        <v>44.018999999999998</v>
+        <v>44.033999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>0.96199999999999997</v>
@@ -4685,7 +4681,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1611.8019999999999</v>
@@ -4717,7 +4713,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>38.012999999999998</v>
@@ -4737,7 +4733,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>40.798000000000002</v>
@@ -4757,7 +4753,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>42.066000000000003</v>
@@ -4777,7 +4773,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.93</v>
@@ -4797,7 +4793,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>38.875</v>
@@ -4817,7 +4813,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0.93500000000000005</v>
@@ -4837,87 +4833,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>1693.04</v>
+        <v>1684.6559999999999</v>
       </c>
       <c r="C11">
-        <v>3049.2339999999999</v>
+        <v>3046.1759999999999</v>
       </c>
       <c r="D11">
-        <v>4577.2150000000001</v>
+        <v>4593.9309999999996</v>
       </c>
       <c r="E11">
-        <v>6170.6180000000004</v>
+        <v>6168.6819999999998</v>
       </c>
       <c r="F11">
-        <v>7775.8440000000001</v>
+        <v>7773.2240000000002</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12">
-        <v>38.750999999999998</v>
+        <v>38.74</v>
       </c>
       <c r="C12">
-        <v>40.418999999999997</v>
+        <v>40.420999999999999</v>
       </c>
       <c r="D12">
-        <v>41.293999999999997</v>
+        <v>41.302999999999997</v>
       </c>
       <c r="E12">
-        <v>41.802999999999997</v>
+        <v>41.805</v>
       </c>
       <c r="F12">
-        <v>42.133000000000003</v>
+        <v>42.134</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <v>41.704999999999998</v>
+        <v>41.698999999999998</v>
       </c>
       <c r="C13">
         <v>42.718000000000004</v>
       </c>
       <c r="D13">
-        <v>43.351999999999997</v>
+        <v>43.359000000000002</v>
       </c>
       <c r="E13">
-        <v>43.767000000000003</v>
+        <v>43.768000000000001</v>
       </c>
       <c r="F13">
-        <v>44.082000000000001</v>
+        <v>44.081000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
-        <v>42.735999999999997</v>
+        <v>42.741999999999997</v>
       </c>
       <c r="C14">
-        <v>44.036999999999999</v>
+        <v>44.033000000000001</v>
       </c>
       <c r="D14">
-        <v>44.923000000000002</v>
+        <v>44.927</v>
       </c>
       <c r="E14">
-        <v>45.564</v>
+        <v>45.567</v>
       </c>
       <c r="F14">
-        <v>46.034999999999997</v>
+        <v>46.033999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>0.93700000000000006</v>
@@ -4937,19 +4933,19 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>39.625</v>
+        <v>39.616</v>
       </c>
       <c r="C16">
-        <v>41.19</v>
+        <v>41.192</v>
       </c>
       <c r="D16">
-        <v>42.036999999999999</v>
+        <v>42.045999999999999</v>
       </c>
       <c r="E16">
-        <v>42.545999999999999</v>
+        <v>42.548000000000002</v>
       </c>
       <c r="F16">
         <v>42.886000000000003</v>
@@ -4957,7 +4953,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>0.94199999999999995</v>
@@ -5024,7 +5020,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1834.664</v>
@@ -5056,7 +5052,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>35.253</v>
@@ -5076,7 +5072,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>38.774000000000001</v>
@@ -5096,7 +5092,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>39.911999999999999</v>
@@ -5116,7 +5112,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.90600000000000003</v>
@@ -5136,7 +5132,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>36.234000000000002</v>
@@ -5156,7 +5152,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0.91</v>
@@ -5176,59 +5172,59 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>1960.0609999999999</v>
+        <v>1959.002</v>
       </c>
       <c r="C11">
-        <v>3416.0010000000002</v>
+        <v>3420.1909999999998</v>
       </c>
       <c r="D11">
-        <v>4942.57</v>
+        <v>4962.3540000000003</v>
       </c>
       <c r="E11">
-        <v>6400.5820000000003</v>
+        <v>6394.2330000000002</v>
       </c>
       <c r="F11">
-        <v>7922.7110000000002</v>
+        <v>7935.7179999999998</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>35.887</v>
       </c>
       <c r="C12">
-        <v>37.595999999999997</v>
+        <v>37.600999999999999</v>
       </c>
       <c r="D12">
-        <v>38.703000000000003</v>
+        <v>38.715000000000003</v>
       </c>
       <c r="E12">
-        <v>39.430999999999997</v>
+        <v>39.433</v>
       </c>
       <c r="F12">
-        <v>39.976999999999997</v>
+        <v>39.987000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <v>40.006</v>
+        <v>39.997</v>
       </c>
       <c r="C13">
-        <v>41.069000000000003</v>
+        <v>41.067</v>
       </c>
       <c r="D13">
-        <v>41.820999999999998</v>
+        <v>41.823</v>
       </c>
       <c r="E13">
-        <v>42.32</v>
+        <v>42.319000000000003</v>
       </c>
       <c r="F13">
         <v>42.691000000000003</v>
@@ -5236,27 +5232,27 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
-        <v>40.826999999999998</v>
+        <v>40.823</v>
       </c>
       <c r="C14">
-        <v>41.956000000000003</v>
+        <v>41.957000000000001</v>
       </c>
       <c r="D14">
-        <v>42.893999999999998</v>
+        <v>42.905999999999999</v>
       </c>
       <c r="E14">
-        <v>43.581000000000003</v>
+        <v>43.576000000000001</v>
       </c>
       <c r="F14">
-        <v>44.116999999999997</v>
+        <v>44.122</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>0.91700000000000004</v>
@@ -5265,7 +5261,7 @@
         <v>0.93899999999999995</v>
       </c>
       <c r="D15">
-        <v>0.94899999999999995</v>
+        <v>0.95</v>
       </c>
       <c r="E15">
         <v>0.95499999999999996</v>
@@ -5276,27 +5272,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>36.94</v>
+        <v>36.939</v>
       </c>
       <c r="C16">
-        <v>38.551000000000002</v>
+        <v>38.555</v>
       </c>
       <c r="D16">
-        <v>39.61</v>
+        <v>39.621000000000002</v>
       </c>
       <c r="E16">
-        <v>40.311</v>
+        <v>40.313000000000002</v>
       </c>
       <c r="F16">
-        <v>40.838000000000001</v>
+        <v>40.845999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>0.92300000000000004</v>
@@ -5363,7 +5359,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>2012.836</v>
@@ -5395,7 +5391,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>35.896000000000001</v>
@@ -5415,7 +5411,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>40.999000000000002</v>
@@ -5435,7 +5431,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>40.970999999999997</v>
@@ -5455,7 +5451,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5475,7 +5471,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>37.030999999999999</v>
@@ -5495,7 +5491,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0.91300000000000003</v>
@@ -5515,67 +5511,67 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>2004.675</v>
+        <v>2005.1369999999999</v>
       </c>
       <c r="C11">
-        <v>3506.422</v>
+        <v>3503.558</v>
       </c>
       <c r="D11">
-        <v>5006.317</v>
+        <v>5004.6000000000004</v>
       </c>
       <c r="E11">
-        <v>6557.3209999999999</v>
+        <v>6520.0439999999999</v>
       </c>
       <c r="F11">
-        <v>8060.5559999999996</v>
+        <v>8070.683</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12">
-        <v>36.28</v>
+        <v>36.283000000000001</v>
       </c>
       <c r="C12">
-        <v>37.585000000000001</v>
+        <v>37.584000000000003</v>
       </c>
       <c r="D12">
-        <v>38.209000000000003</v>
+        <v>38.210999999999999</v>
       </c>
       <c r="E12">
-        <v>38.593000000000004</v>
+        <v>38.594000000000001</v>
       </c>
       <c r="F12">
-        <v>38.853000000000002</v>
+        <v>38.856999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <v>42.042000000000002</v>
+        <v>42.042999999999999</v>
       </c>
       <c r="C13">
-        <v>42.966999999999999</v>
+        <v>42.966000000000001</v>
       </c>
       <c r="D13">
-        <v>43.423000000000002</v>
+        <v>43.420999999999999</v>
       </c>
       <c r="E13">
-        <v>43.68</v>
+        <v>43.674999999999997</v>
       </c>
       <c r="F13">
-        <v>43.843000000000004</v>
+        <v>43.847000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>42.405999999999999</v>
@@ -5584,18 +5580,18 @@
         <v>43.78</v>
       </c>
       <c r="D14">
-        <v>44.497</v>
+        <v>44.500999999999998</v>
       </c>
       <c r="E14">
-        <v>44.906999999999996</v>
+        <v>44.902999999999999</v>
       </c>
       <c r="F14">
-        <v>45.168999999999997</v>
+        <v>45.170999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5610,32 +5606,32 @@
         <v>0.92900000000000005</v>
       </c>
       <c r="F15">
-        <v>0.93100000000000005</v>
+        <v>0.93200000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>37.520000000000003</v>
+        <v>37.523000000000003</v>
       </c>
       <c r="C16">
-        <v>38.805999999999997</v>
+        <v>38.805</v>
       </c>
       <c r="D16">
-        <v>39.423999999999999</v>
+        <v>39.426000000000002</v>
       </c>
       <c r="E16">
         <v>39.801000000000002</v>
       </c>
       <c r="F16">
-        <v>40.054000000000002</v>
+        <v>40.057000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>0.92100000000000004</v>
@@ -5664,9 +5660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5704,7 +5698,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1984.951</v>
@@ -5736,7 +5730,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>34.497</v>
@@ -5756,7 +5750,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>40.106999999999999</v>
@@ -5776,7 +5770,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>42.6</v>
@@ -5796,7 +5790,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5816,7 +5810,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>35.814999999999998</v>
@@ -5836,7 +5830,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0.90900000000000003</v>
@@ -5856,79 +5850,79 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>1980.1220000000001</v>
+        <v>1979.3810000000001</v>
       </c>
       <c r="C11">
-        <v>3479.384</v>
+        <v>3479.8580000000002</v>
       </c>
       <c r="D11">
-        <v>5122.4319999999998</v>
+        <v>5143.9960000000001</v>
       </c>
       <c r="E11">
-        <v>6738.0659999999998</v>
+        <v>6669.9210000000003</v>
       </c>
       <c r="F11">
-        <v>8322.4959999999992</v>
+        <v>8318.8340000000007</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12">
-        <v>34.912999999999997</v>
+        <v>34.917000000000002</v>
       </c>
       <c r="C12">
-        <v>35.337000000000003</v>
+        <v>35.341999999999999</v>
       </c>
       <c r="D12">
-        <v>35.603999999999999</v>
+        <v>35.612000000000002</v>
       </c>
       <c r="E12">
-        <v>35.807000000000002</v>
+        <v>35.805</v>
       </c>
       <c r="F12">
-        <v>35.969000000000001</v>
+        <v>35.975000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <v>40.969000000000001</v>
+        <v>40.963000000000001</v>
       </c>
       <c r="C13">
-        <v>41.337000000000003</v>
+        <v>41.326000000000001</v>
       </c>
       <c r="D13">
-        <v>41.613999999999997</v>
+        <v>41.61</v>
       </c>
       <c r="E13">
-        <v>41.831000000000003</v>
+        <v>41.823999999999998</v>
       </c>
       <c r="F13">
-        <v>41.965000000000003</v>
+        <v>41.963999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
-        <v>43.220999999999997</v>
+        <v>43.212000000000003</v>
       </c>
       <c r="C14">
-        <v>43.526000000000003</v>
+        <v>43.512999999999998</v>
       </c>
       <c r="D14">
-        <v>43.764000000000003</v>
+        <v>43.753999999999998</v>
       </c>
       <c r="E14">
-        <v>43.978000000000002</v>
+        <v>43.970999999999997</v>
       </c>
       <c r="F14">
         <v>44.116999999999997</v>
@@ -5936,7 +5930,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5951,32 +5945,32 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="F15">
-        <v>0.91300000000000003</v>
+        <v>0.91400000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>36.264000000000003</v>
+        <v>36.267000000000003</v>
       </c>
       <c r="C16">
-        <v>36.680999999999997</v>
+        <v>36.683999999999997</v>
       </c>
       <c r="D16">
-        <v>36.947000000000003</v>
+        <v>36.954000000000001</v>
       </c>
       <c r="E16">
-        <v>37.152000000000001</v>
+        <v>37.149000000000001</v>
       </c>
       <c r="F16">
-        <v>37.311</v>
+        <v>37.317</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>0.91600000000000004</v>
@@ -6005,7 +5999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6032,18 +6026,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1960.646</v>
@@ -6064,18 +6058,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>35.564999999999998</v>
@@ -6095,7 +6089,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>38.436</v>
@@ -6115,7 +6109,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>40.572000000000003</v>
@@ -6135,7 +6129,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6">
         <v>0.9</v>
@@ -6155,7 +6149,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>36.505000000000003</v>
@@ -6175,7 +6169,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0.90700000000000003</v>
@@ -6195,87 +6189,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>1987.9860000000001</v>
+        <v>1986.5650000000001</v>
       </c>
       <c r="C11">
-        <v>3478.125</v>
+        <v>3477.07</v>
       </c>
       <c r="D11">
-        <v>4973.3010000000004</v>
+        <v>4969.9359999999997</v>
       </c>
       <c r="E11">
-        <v>6474.9139999999998</v>
+        <v>6474.2889999999998</v>
       </c>
       <c r="F11">
-        <v>7915.268</v>
+        <v>7965.0370000000003</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12">
-        <v>36.14</v>
+        <v>36.140999999999998</v>
       </c>
       <c r="C12">
         <v>37.273000000000003</v>
       </c>
       <c r="D12">
-        <v>37.771000000000001</v>
+        <v>37.771999999999998</v>
       </c>
       <c r="E12">
-        <v>38.052</v>
+        <v>38.054000000000002</v>
       </c>
       <c r="F12">
-        <v>38.234000000000002</v>
+        <v>38.241</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <v>39.087000000000003</v>
+        <v>39.090000000000003</v>
       </c>
       <c r="C13">
-        <v>39.567999999999998</v>
+        <v>39.57</v>
       </c>
       <c r="D13">
-        <v>39.82</v>
+        <v>39.819000000000003</v>
       </c>
       <c r="E13">
-        <v>39.994</v>
+        <v>39.996000000000002</v>
       </c>
       <c r="F13">
-        <v>40.124000000000002</v>
+        <v>40.128999999999998</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14">
-        <v>41.698</v>
+        <v>41.695999999999998</v>
       </c>
       <c r="C14">
-        <v>42.631999999999998</v>
+        <v>42.634999999999998</v>
       </c>
       <c r="D14">
-        <v>43.148000000000003</v>
+        <v>43.154000000000003</v>
       </c>
       <c r="E14">
-        <v>43.488</v>
+        <v>43.485999999999997</v>
       </c>
       <c r="F14">
-        <v>43.722999999999999</v>
+        <v>43.731999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>0.90800000000000003</v>
@@ -6295,27 +6289,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <v>37.122</v>
+        <v>37.124000000000002</v>
       </c>
       <c r="C16">
         <v>38.17</v>
       </c>
       <c r="D16">
-        <v>38.637999999999998</v>
+        <v>38.639000000000003</v>
       </c>
       <c r="E16">
-        <v>38.908999999999999</v>
+        <v>38.911000000000001</v>
       </c>
       <c r="F16">
-        <v>39.087000000000003</v>
+        <v>39.094000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>0.91700000000000004</v>

</xml_diff>

<commit_message>
vvc: 1. refine chroma lambda. 2. decrease bdrate by 0.2%. 3. update vvc performance data.
</commit_message>
<xml_diff>
--- a/doc/xin266vsx265.xlsx
+++ b/doc/xin266vsx265.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\xin26x-github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47E87F2-4BBD-4E77-90ED-21C504CF1C8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B9239-B0ED-4E40-BACA-4410A1F2C6CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="60">
   <si>
     <t>bd_psnr{XIN266}/{X265}</t>
   </si>
@@ -61,16 +61,37 @@
     <t>8000000</t>
   </si>
   <si>
+    <t>testRATE</t>
+  </si>
+  <si>
+    <t>testYPSNR</t>
+  </si>
+  <si>
+    <t>testUPSNR</t>
+  </si>
+  <si>
+    <t>testVPSNR</t>
+  </si>
+  <si>
+    <t>testYSSIM</t>
+  </si>
+  <si>
+    <t>testgPSNR</t>
+  </si>
+  <si>
+    <t>testgSSIM</t>
+  </si>
+  <si>
     <t>0.41</t>
   </si>
   <si>
-    <t>-19.84</t>
+    <t>-19.59</t>
   </si>
   <si>
     <t>0.46</t>
   </si>
   <si>
-    <t>-22.04</t>
+    <t>-22.05</t>
   </si>
   <si>
     <t>B_Kimono1_1920x1080_24</t>
@@ -79,13 +100,13 @@
     <t>0.44</t>
   </si>
   <si>
-    <t>-16.94</t>
+    <t>-16.91</t>
   </si>
   <si>
     <t>0.47</t>
   </si>
   <si>
-    <t>-18.54</t>
+    <t>-18.74</t>
   </si>
   <si>
     <t>B_ParkScene_1920x1080_24</t>
@@ -94,13 +115,13 @@
     <t>0.43</t>
   </si>
   <si>
-    <t>-13.44</t>
+    <t>-13.45</t>
   </si>
   <si>
-    <t>0.49</t>
+    <t>0.5</t>
   </si>
   <si>
-    <t>-15.77</t>
+    <t>-16.02</t>
   </si>
   <si>
     <t>B_BasketballDrive_1920x1080_50</t>
@@ -109,13 +130,13 @@
     <t>0.27</t>
   </si>
   <si>
-    <t>-13.13</t>
+    <t>-12.94</t>
   </si>
   <si>
     <t>0.36</t>
   </si>
   <si>
-    <t>-16.83</t>
+    <t>-16.9</t>
   </si>
   <si>
     <t>B_BQTerrace_1920x1080_60</t>
@@ -124,22 +145,25 @@
     <t>0.31</t>
   </si>
   <si>
-    <t>-30.95</t>
+    <t>-30.84</t>
   </si>
   <si>
     <t>0.33</t>
   </si>
   <si>
-    <t>-31.95</t>
+    <t>-32.16</t>
   </si>
   <si>
     <t>B_Cactus_1920x1080_50</t>
   </si>
   <si>
-    <t>-23.07</t>
+    <t>0.42</t>
   </si>
   <si>
-    <t>-25.87</t>
+    <t>-22.89</t>
+  </si>
+  <si>
+    <t>-26.07</t>
   </si>
   <si>
     <t>x265RATE</t>
@@ -341,7 +365,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FEA6-47D1-B165-01BE171BE0A9}"/>
+              <c16:uniqueId val="{00000000-5082-4B38-B6F8-0ADB0DEDF815}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -370,19 +394,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1980.2940000000001</c:v>
+                  <c:v>1979.5830000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3456.6660000000002</c:v>
+                  <c:v>3468.1219999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4952.009</c:v>
+                  <c:v>4949.857</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6455.8519999999999</c:v>
+                  <c:v>6437.558</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8009.3339999999998</c:v>
+                  <c:v>7995.3590000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,19 +418,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41.779000000000003</c:v>
+                  <c:v>41.786000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.973999999999997</c:v>
+                  <c:v>42.982999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.506999999999998</c:v>
+                  <c:v>43.511000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.808999999999997</c:v>
+                  <c:v>43.813000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.033999999999999</c:v>
+                  <c:v>44.029000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,7 +438,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FEA6-47D1-B165-01BE171BE0A9}"/>
+              <c16:uniqueId val="{00000001-5082-4B38-B6F8-0ADB0DEDF815}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -603,7 +627,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-51B5-4A1E-B10D-F0544BABC22A}"/>
+              <c16:uniqueId val="{00000000-3D96-4D22-B2A2-38627CBE45FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -632,19 +656,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1979.3810000000001</c:v>
+                  <c:v>1979.6859999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3479.8580000000002</c:v>
+                  <c:v>3482.3560000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5143.9960000000001</c:v>
+                  <c:v>5147.6049999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6669.9210000000003</c:v>
+                  <c:v>6668.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8318.8340000000007</c:v>
+                  <c:v>8327.1810000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,7 +700,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-51B5-4A1E-B10D-F0544BABC22A}"/>
+              <c16:uniqueId val="{00000001-3D96-4D22-B2A2-38627CBE45FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -864,7 +888,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-124F-4612-8B04-F154111548CC}"/>
+              <c16:uniqueId val="{00000000-7CA9-4715-9CEC-109D66A339ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -893,19 +917,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1986.5650000000001</c:v>
+                  <c:v>1986.807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3477.07</c:v>
+                  <c:v>3473.232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4969.9359999999997</c:v>
+                  <c:v>4952.0559999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6474.2889999999998</c:v>
+                  <c:v>6456.8239999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7965.0370000000003</c:v>
+                  <c:v>7943.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,19 +941,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.124000000000002</c:v>
+                  <c:v>37.131</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.17</c:v>
+                  <c:v>38.170999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.639000000000003</c:v>
+                  <c:v>38.634</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.911000000000001</c:v>
+                  <c:v>38.906999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.094000000000001</c:v>
+                  <c:v>39.091999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -937,7 +961,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-124F-4612-8B04-F154111548CC}"/>
+              <c16:uniqueId val="{00000001-7CA9-4715-9CEC-109D66A339ED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1126,7 +1150,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0B67-47E3-BDB4-2B4EE870FCA4}"/>
+              <c16:uniqueId val="{00000000-5780-4935-A160-539011EF96B4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1155,19 +1179,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1986.5650000000001</c:v>
+                  <c:v>1986.807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3477.07</c:v>
+                  <c:v>3473.232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4969.9359999999997</c:v>
+                  <c:v>4952.0559999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6474.2889999999998</c:v>
+                  <c:v>6456.8239999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7965.0370000000003</c:v>
+                  <c:v>7943.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1188,7 +1212,7 @@
                   <c:v>0.93300000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.93500000000000005</c:v>
+                  <c:v>0.93600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.93700000000000006</c:v>
@@ -1199,7 +1223,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0B67-47E3-BDB4-2B4EE870FCA4}"/>
+              <c16:uniqueId val="{00000001-5780-4935-A160-539011EF96B4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1387,7 +1411,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F911-4AAE-91B3-7D342C595075}"/>
+              <c16:uniqueId val="{00000000-3ADC-4070-A981-B2257CD08AD0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1416,19 +1440,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1980.2940000000001</c:v>
+                  <c:v>1979.5830000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3456.6660000000002</c:v>
+                  <c:v>3468.1219999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4952.009</c:v>
+                  <c:v>4949.857</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6455.8519999999999</c:v>
+                  <c:v>6437.558</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8009.3339999999998</c:v>
+                  <c:v>7995.3590000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1460,7 +1484,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F911-4AAE-91B3-7D342C595075}"/>
+              <c16:uniqueId val="{00000001-3ADC-4070-A981-B2257CD08AD0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1648,7 +1672,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-75C7-48C8-A6BA-919745449517}"/>
+              <c16:uniqueId val="{00000000-0890-4567-B49F-88B1AEB677B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1677,19 +1701,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1684.6559999999999</c:v>
+                  <c:v>1694.683</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3046.1759999999999</c:v>
+                  <c:v>3054.7429999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4593.9309999999996</c:v>
+                  <c:v>4564.6719999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6168.6819999999998</c:v>
+                  <c:v>6169.3270000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7773.2240000000002</c:v>
+                  <c:v>7782.5370000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,19 +1725,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.616</c:v>
+                  <c:v>39.640999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.192</c:v>
+                  <c:v>41.204000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.045999999999999</c:v>
+                  <c:v>42.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.548000000000002</c:v>
+                  <c:v>42.55</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.886000000000003</c:v>
+                  <c:v>42.890999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,7 +1745,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-75C7-48C8-A6BA-919745449517}"/>
+              <c16:uniqueId val="{00000001-0890-4567-B49F-88B1AEB677B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1910,7 +1934,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2C15-48AC-B1D2-E0DCBF1D4B51}"/>
+              <c16:uniqueId val="{00000000-93CF-42C8-8040-8C395A4F1355}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1939,19 +1963,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1684.6559999999999</c:v>
+                  <c:v>1694.683</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3046.1759999999999</c:v>
+                  <c:v>3054.7429999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4593.9309999999996</c:v>
+                  <c:v>4564.6719999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6168.6819999999998</c:v>
+                  <c:v>6169.3270000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7773.2240000000002</c:v>
+                  <c:v>7782.5370000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1983,7 +2007,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2C15-48AC-B1D2-E0DCBF1D4B51}"/>
+              <c16:uniqueId val="{00000001-93CF-42C8-8040-8C395A4F1355}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2171,7 +2195,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-31B7-419A-9E7F-9D931CD07E70}"/>
+              <c16:uniqueId val="{00000000-82D9-439B-AABB-5369EC2C4F53}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2200,19 +2224,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1959.002</c:v>
+                  <c:v>1958.4349999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3420.1909999999998</c:v>
+                  <c:v>3420.1039999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4962.3540000000003</c:v>
+                  <c:v>4916.0770000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6394.2330000000002</c:v>
+                  <c:v>6403.6580000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7935.7179999999998</c:v>
+                  <c:v>7897.9560000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2224,19 +2248,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.939</c:v>
+                  <c:v>36.950000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.555</c:v>
+                  <c:v>38.563000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.621000000000002</c:v>
+                  <c:v>39.604999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.313000000000002</c:v>
+                  <c:v>40.319000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.845999999999997</c:v>
+                  <c:v>40.838999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,7 +2268,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-31B7-419A-9E7F-9D931CD07E70}"/>
+              <c16:uniqueId val="{00000001-82D9-439B-AABB-5369EC2C4F53}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2433,7 +2457,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F249-42FA-B193-697FF63C25BB}"/>
+              <c16:uniqueId val="{00000000-0654-4AE3-8807-3872953E05DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2462,19 +2486,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1959.002</c:v>
+                  <c:v>1958.4349999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3420.1909999999998</c:v>
+                  <c:v>3420.1039999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4962.3540000000003</c:v>
+                  <c:v>4916.0770000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6394.2330000000002</c:v>
+                  <c:v>6403.6580000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7935.7179999999998</c:v>
+                  <c:v>7897.9560000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2506,7 +2530,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F249-42FA-B193-697FF63C25BB}"/>
+              <c16:uniqueId val="{00000001-0654-4AE3-8807-3872953E05DE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2694,7 +2718,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-571E-4F84-8C2B-1ADC36D8F9D9}"/>
+              <c16:uniqueId val="{00000000-F5EC-4B4F-9BCD-059E4808EE2B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2707,7 +2731,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>xin266gPSNR</c:v>
+                  <c:v>testgPSNR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2723,19 +2747,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2005.1369999999999</c:v>
+                  <c:v>2000.2470000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3503.558</c:v>
+                  <c:v>3508.6239999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5004.6000000000004</c:v>
+                  <c:v>5006.8100000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6520.0439999999999</c:v>
+                  <c:v>6524.6260000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8070.683</c:v>
+                  <c:v>8072.7349999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2747,19 +2771,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.523000000000003</c:v>
+                  <c:v>37.526000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.805</c:v>
+                  <c:v>38.804000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.426000000000002</c:v>
+                  <c:v>39.429000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.801000000000002</c:v>
+                  <c:v>39.798999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.057000000000002</c:v>
+                  <c:v>40.067</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2767,7 +2791,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-571E-4F84-8C2B-1ADC36D8F9D9}"/>
+              <c16:uniqueId val="{00000001-F5EC-4B4F-9BCD-059E4808EE2B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2956,7 +2980,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6AEC-4607-A43E-1819078A1B26}"/>
+              <c16:uniqueId val="{00000000-45BA-4622-901B-845AD8A7F012}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2969,7 +2993,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>xin266gSSIM</c:v>
+                  <c:v>testgSSIM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2985,19 +3009,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2005.1369999999999</c:v>
+                  <c:v>2000.2470000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3503.558</c:v>
+                  <c:v>3508.6239999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5004.6000000000004</c:v>
+                  <c:v>5006.8100000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6520.0439999999999</c:v>
+                  <c:v>6524.6260000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8070.683</c:v>
+                  <c:v>8072.7349999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3029,7 +3053,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6AEC-4607-A43E-1819078A1B26}"/>
+              <c16:uniqueId val="{00000001-45BA-4622-901B-845AD8A7F012}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3217,7 +3241,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-24C4-4E85-8822-A04F47C23AEC}"/>
+              <c16:uniqueId val="{00000000-EE92-41EB-8171-FA07E9E6B853}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3246,19 +3270,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1979.3810000000001</c:v>
+                  <c:v>1979.6859999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3479.8580000000002</c:v>
+                  <c:v>3482.3560000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5143.9960000000001</c:v>
+                  <c:v>5147.6049999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6669.9210000000003</c:v>
+                  <c:v>6668.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8318.8340000000007</c:v>
+                  <c:v>8327.1810000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3270,19 +3294,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.267000000000003</c:v>
+                  <c:v>36.274000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.683999999999997</c:v>
+                  <c:v>36.686999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.954000000000001</c:v>
+                  <c:v>36.956000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.149000000000001</c:v>
+                  <c:v>37.151000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.317</c:v>
+                  <c:v>37.319000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3290,7 +3314,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-24C4-4E85-8822-A04F47C23AEC}"/>
+              <c16:uniqueId val="{00000001-EE92-41EB-8171-FA07E9E6B853}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4176,7 +4200,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -4186,19 +4210,19 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4221,7 +4245,7 @@
         <v>0.31</v>
       </c>
       <c r="G2">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4229,22 +4253,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-19.84</v>
+        <v>-19.59</v>
       </c>
       <c r="C3">
-        <v>-16.940000000000001</v>
+        <v>-16.91</v>
       </c>
       <c r="D3">
-        <v>-13.44</v>
+        <v>-13.45</v>
       </c>
       <c r="E3">
-        <v>-13.13</v>
+        <v>-12.94</v>
       </c>
       <c r="F3">
-        <v>-30.95</v>
+        <v>-30.84</v>
       </c>
       <c r="G3">
-        <v>-23.07</v>
+        <v>-22.89</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4258,7 +4282,7 @@
         <v>0.47</v>
       </c>
       <c r="D4">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
         <v>0.36</v>
@@ -4275,22 +4299,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-22.04</v>
+        <v>-22.05</v>
       </c>
       <c r="C5">
-        <v>-18.54</v>
+        <v>-18.739999999999998</v>
       </c>
       <c r="D5">
-        <v>-15.77</v>
+        <v>-16.02</v>
       </c>
       <c r="E5">
-        <v>-16.829999999999998</v>
+        <v>-16.899999999999999</v>
       </c>
       <c r="F5">
-        <v>-31.95</v>
+        <v>-32.159999999999997</v>
       </c>
       <c r="G5">
-        <v>-25.87</v>
+        <v>-26.07</v>
       </c>
     </row>
   </sheetData>
@@ -4331,18 +4355,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>1947.596</v>
@@ -4363,18 +4387,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>39.904000000000003</v>
@@ -4394,7 +4418,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>43.831000000000003</v>
@@ -4414,7 +4438,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>45.2</v>
@@ -4434,7 +4458,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>0.94799999999999995</v>
@@ -4454,7 +4478,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>40.963999999999999</v>
@@ -4474,7 +4498,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0.95599999999999996</v>
@@ -4494,87 +4518,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B11">
-        <v>1980.2940000000001</v>
+        <v>1979.5830000000001</v>
       </c>
       <c r="C11">
-        <v>3456.6660000000002</v>
+        <v>3468.1219999999998</v>
       </c>
       <c r="D11">
-        <v>4952.009</v>
+        <v>4949.857</v>
       </c>
       <c r="E11">
-        <v>6455.8519999999999</v>
+        <v>6437.558</v>
       </c>
       <c r="F11">
-        <v>8009.3339999999998</v>
+        <v>7995.3590000000004</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B12">
-        <v>40.654000000000003</v>
+        <v>40.655999999999999</v>
       </c>
       <c r="C12">
-        <v>41.874000000000002</v>
+        <v>41.877000000000002</v>
       </c>
       <c r="D12">
-        <v>42.415999999999997</v>
+        <v>42.414999999999999</v>
       </c>
       <c r="E12">
         <v>42.719000000000001</v>
       </c>
       <c r="F12">
-        <v>42.944000000000003</v>
+        <v>42.935000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>44.99</v>
+        <v>45.021999999999998</v>
       </c>
       <c r="C13">
-        <v>45.957999999999998</v>
+        <v>45.996000000000002</v>
       </c>
       <c r="D13">
-        <v>46.402999999999999</v>
+        <v>46.436999999999998</v>
       </c>
       <c r="E13">
-        <v>46.682000000000002</v>
+        <v>46.707999999999998</v>
       </c>
       <c r="F13">
-        <v>46.896999999999998</v>
+        <v>46.915999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>46.47</v>
+        <v>46.503</v>
       </c>
       <c r="C14">
-        <v>47.603999999999999</v>
+        <v>47.665999999999997</v>
       </c>
       <c r="D14">
-        <v>48.127000000000002</v>
+        <v>48.165999999999997</v>
       </c>
       <c r="E14">
-        <v>48.45</v>
+        <v>48.487000000000002</v>
       </c>
       <c r="F14">
-        <v>48.694000000000003</v>
+        <v>48.718000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0.95399999999999996</v>
@@ -4594,27 +4618,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B16">
-        <v>41.779000000000003</v>
+        <v>41.786000000000001</v>
       </c>
       <c r="C16">
-        <v>42.973999999999997</v>
+        <v>42.982999999999997</v>
       </c>
       <c r="D16">
-        <v>43.506999999999998</v>
+        <v>43.511000000000003</v>
       </c>
       <c r="E16">
-        <v>43.808999999999997</v>
+        <v>43.813000000000002</v>
       </c>
       <c r="F16">
-        <v>44.033999999999999</v>
+        <v>44.029000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0.96199999999999997</v>
@@ -4670,18 +4694,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>1611.8019999999999</v>
@@ -4702,18 +4726,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>38.012999999999998</v>
@@ -4733,7 +4757,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>40.798000000000002</v>
@@ -4753,7 +4777,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>42.066000000000003</v>
@@ -4773,7 +4797,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>0.93</v>
@@ -4793,7 +4817,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>38.875</v>
@@ -4813,7 +4837,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0.93500000000000005</v>
@@ -4833,87 +4857,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B11">
-        <v>1684.6559999999999</v>
+        <v>1694.683</v>
       </c>
       <c r="C11">
-        <v>3046.1759999999999</v>
+        <v>3054.7429999999999</v>
       </c>
       <c r="D11">
-        <v>4593.9309999999996</v>
+        <v>4564.6719999999996</v>
       </c>
       <c r="E11">
-        <v>6168.6819999999998</v>
+        <v>6169.3270000000002</v>
       </c>
       <c r="F11">
-        <v>7773.2240000000002</v>
+        <v>7782.5370000000003</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B12">
-        <v>38.74</v>
+        <v>38.765999999999998</v>
       </c>
       <c r="C12">
-        <v>40.420999999999999</v>
+        <v>40.424999999999997</v>
       </c>
       <c r="D12">
-        <v>41.302999999999997</v>
+        <v>41.289000000000001</v>
       </c>
       <c r="E12">
-        <v>41.805</v>
+        <v>41.801000000000002</v>
       </c>
       <c r="F12">
-        <v>42.134</v>
+        <v>42.134999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>41.698999999999998</v>
+        <v>41.716999999999999</v>
       </c>
       <c r="C13">
-        <v>42.718000000000004</v>
+        <v>42.758000000000003</v>
       </c>
       <c r="D13">
-        <v>43.359000000000002</v>
+        <v>43.383000000000003</v>
       </c>
       <c r="E13">
-        <v>43.768000000000001</v>
+        <v>43.790999999999997</v>
       </c>
       <c r="F13">
-        <v>44.081000000000003</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>42.741999999999997</v>
+        <v>42.765999999999998</v>
       </c>
       <c r="C14">
-        <v>44.033000000000001</v>
+        <v>44.088000000000001</v>
       </c>
       <c r="D14">
-        <v>44.927</v>
+        <v>44.957000000000001</v>
       </c>
       <c r="E14">
-        <v>45.567</v>
+        <v>45.595999999999997</v>
       </c>
       <c r="F14">
-        <v>46.033999999999999</v>
+        <v>46.058999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0.93700000000000006</v>
@@ -4933,27 +4957,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B16">
-        <v>39.616</v>
+        <v>39.640999999999998</v>
       </c>
       <c r="C16">
-        <v>41.192</v>
+        <v>41.204000000000001</v>
       </c>
       <c r="D16">
-        <v>42.045999999999999</v>
+        <v>42.04</v>
       </c>
       <c r="E16">
-        <v>42.548000000000002</v>
+        <v>42.55</v>
       </c>
       <c r="F16">
-        <v>42.886000000000003</v>
+        <v>42.890999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0.94199999999999995</v>
@@ -5009,18 +5033,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>1834.664</v>
@@ -5041,18 +5065,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>35.253</v>
@@ -5072,7 +5096,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>38.774000000000001</v>
@@ -5092,7 +5116,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>39.911999999999999</v>
@@ -5112,7 +5136,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>0.90600000000000003</v>
@@ -5132,7 +5156,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>36.234000000000002</v>
@@ -5152,7 +5176,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0.91</v>
@@ -5172,87 +5196,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B11">
-        <v>1959.002</v>
+        <v>1958.4349999999999</v>
       </c>
       <c r="C11">
-        <v>3420.1909999999998</v>
+        <v>3420.1039999999998</v>
       </c>
       <c r="D11">
-        <v>4962.3540000000003</v>
+        <v>4916.0770000000002</v>
       </c>
       <c r="E11">
-        <v>6394.2330000000002</v>
+        <v>6403.6580000000004</v>
       </c>
       <c r="F11">
-        <v>7935.7179999999998</v>
+        <v>7897.9560000000001</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <v>35.887</v>
       </c>
       <c r="C12">
-        <v>37.600999999999999</v>
+        <v>37.6</v>
       </c>
       <c r="D12">
-        <v>38.715000000000003</v>
+        <v>38.691000000000003</v>
       </c>
       <c r="E12">
         <v>39.433</v>
       </c>
       <c r="F12">
-        <v>39.987000000000002</v>
+        <v>39.973999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>39.997</v>
+        <v>40.061</v>
       </c>
       <c r="C13">
-        <v>41.067</v>
+        <v>41.116999999999997</v>
       </c>
       <c r="D13">
-        <v>41.823</v>
+        <v>41.847000000000001</v>
       </c>
       <c r="E13">
-        <v>42.319000000000003</v>
+        <v>42.353000000000002</v>
       </c>
       <c r="F13">
-        <v>42.691000000000003</v>
+        <v>42.713999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>40.823</v>
+        <v>40.908000000000001</v>
       </c>
       <c r="C14">
-        <v>41.957000000000001</v>
+        <v>42.01</v>
       </c>
       <c r="D14">
-        <v>42.905999999999999</v>
+        <v>42.918999999999997</v>
       </c>
       <c r="E14">
-        <v>43.576000000000001</v>
+        <v>43.610999999999997</v>
       </c>
       <c r="F14">
-        <v>44.122</v>
+        <v>44.133000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0.91700000000000004</v>
@@ -5261,7 +5285,7 @@
         <v>0.93899999999999995</v>
       </c>
       <c r="D15">
-        <v>0.95</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="E15">
         <v>0.95499999999999996</v>
@@ -5272,27 +5296,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B16">
-        <v>36.939</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="C16">
-        <v>38.555</v>
+        <v>38.563000000000002</v>
       </c>
       <c r="D16">
-        <v>39.621000000000002</v>
+        <v>39.604999999999997</v>
       </c>
       <c r="E16">
-        <v>40.313000000000002</v>
+        <v>40.319000000000003</v>
       </c>
       <c r="F16">
-        <v>40.845999999999997</v>
+        <v>40.838999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0.92300000000000004</v>
@@ -5348,18 +5372,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>2012.836</v>
@@ -5380,18 +5404,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>35.896000000000001</v>
@@ -5411,7 +5435,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>40.999000000000002</v>
@@ -5431,7 +5455,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>40.970999999999997</v>
@@ -5451,7 +5475,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5471,7 +5495,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>37.030999999999999</v>
@@ -5491,7 +5515,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0.91300000000000003</v>
@@ -5511,87 +5535,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>2005.1369999999999</v>
+        <v>2000.2470000000001</v>
       </c>
       <c r="C11">
-        <v>3503.558</v>
+        <v>3508.6239999999998</v>
       </c>
       <c r="D11">
-        <v>5004.6000000000004</v>
+        <v>5006.8100000000004</v>
       </c>
       <c r="E11">
-        <v>6520.0439999999999</v>
+        <v>6524.6260000000002</v>
       </c>
       <c r="F11">
-        <v>8070.683</v>
+        <v>8072.7349999999997</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>36.283000000000001</v>
+        <v>36.29</v>
       </c>
       <c r="C12">
-        <v>37.584000000000003</v>
+        <v>37.576000000000001</v>
       </c>
       <c r="D12">
-        <v>38.210999999999999</v>
+        <v>38.207999999999998</v>
       </c>
       <c r="E12">
-        <v>38.594000000000001</v>
+        <v>38.585000000000001</v>
       </c>
       <c r="F12">
-        <v>38.856999999999999</v>
+        <v>38.86</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>42.042999999999999</v>
+        <v>42.027999999999999</v>
       </c>
       <c r="C13">
-        <v>42.966000000000001</v>
+        <v>43.006</v>
       </c>
       <c r="D13">
-        <v>43.420999999999999</v>
+        <v>43.463999999999999</v>
       </c>
       <c r="E13">
-        <v>43.674999999999997</v>
+        <v>43.715000000000003</v>
       </c>
       <c r="F13">
-        <v>43.847000000000001</v>
+        <v>43.887</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>42.405999999999999</v>
+        <v>42.35</v>
       </c>
       <c r="C14">
-        <v>43.78</v>
+        <v>43.838000000000001</v>
       </c>
       <c r="D14">
-        <v>44.500999999999998</v>
+        <v>44.564</v>
       </c>
       <c r="E14">
-        <v>44.902999999999999</v>
+        <v>44.970999999999997</v>
       </c>
       <c r="F14">
-        <v>45.170999999999999</v>
+        <v>45.25</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5603,7 +5627,7 @@
         <v>0.92400000000000004</v>
       </c>
       <c r="E15">
-        <v>0.92900000000000005</v>
+        <v>0.92800000000000005</v>
       </c>
       <c r="F15">
         <v>0.93200000000000005</v>
@@ -5611,27 +5635,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>37.523000000000003</v>
+        <v>37.526000000000003</v>
       </c>
       <c r="C16">
-        <v>38.805</v>
+        <v>38.804000000000002</v>
       </c>
       <c r="D16">
-        <v>39.426000000000002</v>
+        <v>39.429000000000002</v>
       </c>
       <c r="E16">
-        <v>39.801000000000002</v>
+        <v>39.798999999999999</v>
       </c>
       <c r="F16">
-        <v>40.057000000000002</v>
+        <v>40.067</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>0.92100000000000004</v>
@@ -5660,7 +5684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q44" sqref="Q44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5687,18 +5713,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>1984.951</v>
@@ -5719,18 +5745,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>34.497</v>
@@ -5750,7 +5776,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>40.106999999999999</v>
@@ -5770,7 +5796,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>42.6</v>
@@ -5790,7 +5816,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5810,7 +5836,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>35.814999999999998</v>
@@ -5830,7 +5856,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0.90900000000000003</v>
@@ -5850,39 +5876,39 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B11">
-        <v>1979.3810000000001</v>
+        <v>1979.6859999999999</v>
       </c>
       <c r="C11">
-        <v>3479.8580000000002</v>
+        <v>3482.3560000000002</v>
       </c>
       <c r="D11">
-        <v>5143.9960000000001</v>
+        <v>5147.6049999999996</v>
       </c>
       <c r="E11">
-        <v>6669.9210000000003</v>
+        <v>6668.03</v>
       </c>
       <c r="F11">
-        <v>8318.8340000000007</v>
+        <v>8327.1810000000005</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B12">
-        <v>34.917000000000002</v>
+        <v>34.918999999999997</v>
       </c>
       <c r="C12">
-        <v>35.341999999999999</v>
+        <v>35.341000000000001</v>
       </c>
       <c r="D12">
-        <v>35.612000000000002</v>
+        <v>35.610999999999997</v>
       </c>
       <c r="E12">
-        <v>35.805</v>
+        <v>35.804000000000002</v>
       </c>
       <c r="F12">
         <v>35.975000000000001</v>
@@ -5890,47 +5916,47 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>40.963000000000001</v>
+        <v>41.023000000000003</v>
       </c>
       <c r="C13">
-        <v>41.326000000000001</v>
+        <v>41.363</v>
       </c>
       <c r="D13">
-        <v>41.61</v>
+        <v>41.631999999999998</v>
       </c>
       <c r="E13">
-        <v>41.823999999999998</v>
+        <v>41.845999999999997</v>
       </c>
       <c r="F13">
-        <v>41.963999999999999</v>
+        <v>41.994</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>43.212000000000003</v>
+        <v>43.259</v>
       </c>
       <c r="C14">
-        <v>43.512999999999998</v>
+        <v>43.546999999999997</v>
       </c>
       <c r="D14">
-        <v>43.753999999999998</v>
+        <v>43.792999999999999</v>
       </c>
       <c r="E14">
-        <v>43.970999999999997</v>
+        <v>43.993000000000002</v>
       </c>
       <c r="F14">
-        <v>44.116999999999997</v>
+        <v>44.145000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5950,27 +5976,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B16">
-        <v>36.267000000000003</v>
+        <v>36.274000000000001</v>
       </c>
       <c r="C16">
-        <v>36.683999999999997</v>
+        <v>36.686999999999998</v>
       </c>
       <c r="D16">
-        <v>36.954000000000001</v>
+        <v>36.956000000000003</v>
       </c>
       <c r="E16">
-        <v>37.149000000000001</v>
+        <v>37.151000000000003</v>
       </c>
       <c r="F16">
-        <v>37.317</v>
+        <v>37.319000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0.91600000000000004</v>
@@ -6026,18 +6052,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>1960.646</v>
@@ -6058,18 +6084,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>35.564999999999998</v>
@@ -6089,7 +6115,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>38.436</v>
@@ -6109,7 +6135,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>40.572000000000003</v>
@@ -6129,7 +6155,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>0.9</v>
@@ -6149,7 +6175,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>36.505000000000003</v>
@@ -6169,7 +6195,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>0.90700000000000003</v>
@@ -6189,87 +6215,87 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B11">
-        <v>1986.5650000000001</v>
+        <v>1986.807</v>
       </c>
       <c r="C11">
-        <v>3477.07</v>
+        <v>3473.232</v>
       </c>
       <c r="D11">
-        <v>4969.9359999999997</v>
+        <v>4952.0559999999996</v>
       </c>
       <c r="E11">
-        <v>6474.2889999999998</v>
+        <v>6456.8239999999996</v>
       </c>
       <c r="F11">
-        <v>7965.0370000000003</v>
+        <v>7943.57</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B12">
-        <v>36.140999999999998</v>
+        <v>36.143000000000001</v>
       </c>
       <c r="C12">
-        <v>37.273000000000003</v>
+        <v>37.267000000000003</v>
       </c>
       <c r="D12">
-        <v>37.771999999999998</v>
+        <v>37.759</v>
       </c>
       <c r="E12">
-        <v>38.054000000000002</v>
+        <v>38.042000000000002</v>
       </c>
       <c r="F12">
-        <v>38.241</v>
+        <v>38.228000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>39.090000000000003</v>
+        <v>39.116</v>
       </c>
       <c r="C13">
-        <v>39.57</v>
+        <v>39.591999999999999</v>
       </c>
       <c r="D13">
-        <v>39.819000000000003</v>
+        <v>39.844999999999999</v>
       </c>
       <c r="E13">
-        <v>39.996000000000002</v>
+        <v>40.024999999999999</v>
       </c>
       <c r="F13">
-        <v>40.128999999999998</v>
+        <v>40.170999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B14">
-        <v>41.695999999999998</v>
+        <v>41.749000000000002</v>
       </c>
       <c r="C14">
-        <v>42.634999999999998</v>
+        <v>42.691000000000003</v>
       </c>
       <c r="D14">
-        <v>43.154000000000003</v>
+        <v>43.192999999999998</v>
       </c>
       <c r="E14">
-        <v>43.485999999999997</v>
+        <v>43.529000000000003</v>
       </c>
       <c r="F14">
-        <v>43.731999999999999</v>
+        <v>43.771000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>0.90800000000000003</v>
@@ -6289,27 +6315,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B16">
-        <v>37.124000000000002</v>
+        <v>37.131</v>
       </c>
       <c r="C16">
-        <v>38.17</v>
+        <v>38.170999999999999</v>
       </c>
       <c r="D16">
-        <v>38.639000000000003</v>
+        <v>38.634</v>
       </c>
       <c r="E16">
-        <v>38.911000000000001</v>
+        <v>38.906999999999996</v>
       </c>
       <c r="F16">
-        <v>39.094000000000001</v>
+        <v>39.091999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0.91700000000000004</v>
@@ -6321,7 +6347,7 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="E17">
-        <v>0.93500000000000005</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="F17">
         <v>0.93700000000000006</v>

</xml_diff>

<commit_message>
vvc: 1. Decrease bdrate 1.1% 2. support dmvr. 3. update performance data.
</commit_message>
<xml_diff>
--- a/doc/xin266vsx265.xlsx
+++ b/doc/xin266vsx265.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\xin26x-github\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6B9239-B0ED-4E40-BACA-4410A1F2C6CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDA43AC-3011-42C1-9484-A63040A835B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
   <si>
     <t>bd_psnr{XIN266}/{X265}</t>
   </si>
@@ -61,82 +61,58 @@
     <t>8000000</t>
   </si>
   <si>
-    <t>testRATE</t>
-  </si>
-  <si>
-    <t>testYPSNR</t>
-  </si>
-  <si>
-    <t>testUPSNR</t>
-  </si>
-  <si>
-    <t>testVPSNR</t>
-  </si>
-  <si>
-    <t>testYSSIM</t>
-  </si>
-  <si>
-    <t>testgPSNR</t>
-  </si>
-  <si>
-    <t>testgSSIM</t>
-  </si>
-  <si>
     <t>0.41</t>
   </si>
   <si>
-    <t>-19.59</t>
+    <t>-19.88</t>
   </si>
   <si>
     <t>0.46</t>
   </si>
   <si>
-    <t>-22.05</t>
+    <t>-22.38</t>
   </si>
   <si>
     <t>B_Kimono1_1920x1080_24</t>
   </si>
   <si>
-    <t>0.44</t>
+    <t>0.49</t>
   </si>
   <si>
-    <t>-16.91</t>
+    <t>-18.83</t>
   </si>
   <si>
-    <t>0.47</t>
+    <t>0.52</t>
   </si>
   <si>
-    <t>-18.74</t>
+    <t>-20.65</t>
   </si>
   <si>
     <t>B_ParkScene_1920x1080_24</t>
   </si>
   <si>
-    <t>0.43</t>
+    <t>-15.2</t>
   </si>
   <si>
-    <t>-13.45</t>
+    <t>0.56</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>-16.02</t>
+    <t>-17.77</t>
   </si>
   <si>
     <t>B_BasketballDrive_1920x1080_50</t>
   </si>
   <si>
-    <t>0.27</t>
+    <t>0.29</t>
   </si>
   <si>
-    <t>-12.94</t>
+    <t>-14.13</t>
   </si>
   <si>
-    <t>0.36</t>
+    <t>0.38</t>
   </si>
   <si>
-    <t>-16.9</t>
+    <t>-18.05</t>
   </si>
   <si>
     <t>B_BQTerrace_1920x1080_60</t>
@@ -145,25 +121,46 @@
     <t>0.31</t>
   </si>
   <si>
-    <t>-30.84</t>
+    <t>-30.98</t>
   </si>
   <si>
     <t>0.33</t>
   </si>
   <si>
-    <t>-32.16</t>
+    <t>-32.29</t>
   </si>
   <si>
     <t>B_Cactus_1920x1080_50</t>
   </si>
   <si>
-    <t>0.42</t>
+    <t>0.45</t>
   </si>
   <si>
-    <t>-22.89</t>
+    <t>-24.6</t>
   </si>
   <si>
-    <t>-26.07</t>
+    <t>-27.72</t>
+  </si>
+  <si>
+    <t>xin266RATE</t>
+  </si>
+  <si>
+    <t>xin266YPSNR</t>
+  </si>
+  <si>
+    <t>xin266UPSNR</t>
+  </si>
+  <si>
+    <t>xin266VPSNR</t>
+  </si>
+  <si>
+    <t>xin266YSSIM</t>
+  </si>
+  <si>
+    <t>xin266gPSNR</t>
+  </si>
+  <si>
+    <t>xin266gSSIM</t>
   </si>
   <si>
     <t>x265RATE</t>
@@ -185,27 +182,6 @@
   </si>
   <si>
     <t>x265gSSIM</t>
-  </si>
-  <si>
-    <t>xin266RATE</t>
-  </si>
-  <si>
-    <t>xin266YPSNR</t>
-  </si>
-  <si>
-    <t>xin266UPSNR</t>
-  </si>
-  <si>
-    <t>xin266VPSNR</t>
-  </si>
-  <si>
-    <t>xin266YSSIM</t>
-  </si>
-  <si>
-    <t>xin266gPSNR</t>
-  </si>
-  <si>
-    <t>xin266gSSIM</t>
   </si>
 </sst>
 </file>
@@ -365,7 +341,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5082-4B38-B6F8-0ADB0DEDF815}"/>
+              <c16:uniqueId val="{00000000-6B6A-4048-B6AF-DD8C5167CF6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -394,19 +370,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1979.5830000000001</c:v>
+                  <c:v>1979.192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3468.1219999999998</c:v>
+                  <c:v>3459.5880000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4949.857</c:v>
+                  <c:v>4951.4560000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6437.558</c:v>
+                  <c:v>6478.2920000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7995.3590000000004</c:v>
+                  <c:v>7993.6930000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,19 +394,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>41.786000000000001</c:v>
+                  <c:v>41.793999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42.982999999999997</c:v>
+                  <c:v>42.984999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.511000000000003</c:v>
+                  <c:v>43.512</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>43.813000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.029000000000003</c:v>
+                  <c:v>44.027999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,7 +414,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5082-4B38-B6F8-0ADB0DEDF815}"/>
+              <c16:uniqueId val="{00000001-6B6A-4048-B6AF-DD8C5167CF6F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -627,7 +603,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3D96-4D22-B2A2-38627CBE45FF}"/>
+              <c16:uniqueId val="{00000000-3631-43A6-A090-3B9F7574D3CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -656,19 +632,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1979.6859999999999</c:v>
+                  <c:v>1980.694</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3482.3560000000002</c:v>
+                  <c:v>3494.1410000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5147.6049999999996</c:v>
+                  <c:v>5124.3310000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6668.03</c:v>
+                  <c:v>6666.567</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8327.1810000000005</c:v>
+                  <c:v>8322.8310000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -700,7 +676,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3D96-4D22-B2A2-38627CBE45FF}"/>
+              <c16:uniqueId val="{00000001-3631-43A6-A090-3B9F7574D3CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -888,7 +864,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7CA9-4715-9CEC-109D66A339ED}"/>
+              <c16:uniqueId val="{00000000-C57D-4945-9952-124A75C361EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -917,19 +893,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1986.807</c:v>
+                  <c:v>1991.7719999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3473.232</c:v>
+                  <c:v>3466.739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4952.0559999999996</c:v>
+                  <c:v>4937.6760000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6456.8239999999996</c:v>
+                  <c:v>6456.4110000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7943.57</c:v>
+                  <c:v>7928.8059999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -941,19 +917,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.131</c:v>
+                  <c:v>37.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.170999999999999</c:v>
+                  <c:v>38.194000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.634</c:v>
+                  <c:v>38.646999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.906999999999996</c:v>
+                  <c:v>38.914000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.091999999999999</c:v>
+                  <c:v>39.097999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -961,7 +937,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7CA9-4715-9CEC-109D66A339ED}"/>
+              <c16:uniqueId val="{00000001-C57D-4945-9952-124A75C361EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1150,7 +1126,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5780-4935-A160-539011EF96B4}"/>
+              <c16:uniqueId val="{00000000-26DB-43A2-8E23-33CEE1367CC4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1179,19 +1155,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1986.807</c:v>
+                  <c:v>1991.7719999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3473.232</c:v>
+                  <c:v>3466.739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4952.0559999999996</c:v>
+                  <c:v>4937.6760000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6456.8239999999996</c:v>
+                  <c:v>6456.4110000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7943.57</c:v>
+                  <c:v>7928.8059999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1203,7 +1179,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.91700000000000004</c:v>
+                  <c:v>0.91800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.92800000000000005</c:v>
@@ -1223,7 +1199,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5780-4935-A160-539011EF96B4}"/>
+              <c16:uniqueId val="{00000001-26DB-43A2-8E23-33CEE1367CC4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1411,7 +1387,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3ADC-4070-A981-B2257CD08AD0}"/>
+              <c16:uniqueId val="{00000000-5488-416E-A281-92518D5AC7E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1440,19 +1416,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1979.5830000000001</c:v>
+                  <c:v>1979.192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3468.1219999999998</c:v>
+                  <c:v>3459.5880000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4949.857</c:v>
+                  <c:v>4951.4560000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6437.558</c:v>
+                  <c:v>6478.2920000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7995.3590000000004</c:v>
+                  <c:v>7993.6930000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1484,7 +1460,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3ADC-4070-A981-B2257CD08AD0}"/>
+              <c16:uniqueId val="{00000001-5488-416E-A281-92518D5AC7E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1672,7 +1648,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0890-4567-B49F-88B1AEB677B2}"/>
+              <c16:uniqueId val="{00000000-720E-48F6-8DA0-A91ACBB174FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1701,19 +1677,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1694.683</c:v>
+                  <c:v>1687.7760000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3054.7429999999999</c:v>
+                  <c:v>3038.3829999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4564.6719999999996</c:v>
+                  <c:v>4544.3850000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6169.3270000000002</c:v>
+                  <c:v>6168.4139999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7782.5370000000003</c:v>
+                  <c:v>7814.0439999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1725,19 +1701,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.640999999999998</c:v>
+                  <c:v>39.731000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.204000000000001</c:v>
+                  <c:v>41.246000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.04</c:v>
+                  <c:v>42.061</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42.55</c:v>
+                  <c:v>42.569000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.890999999999998</c:v>
+                  <c:v>42.905999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1745,7 +1721,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0890-4567-B49F-88B1AEB677B2}"/>
+              <c16:uniqueId val="{00000001-720E-48F6-8DA0-A91ACBB174FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1934,7 +1910,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-93CF-42C8-8040-8C395A4F1355}"/>
+              <c16:uniqueId val="{00000000-C495-48D9-A0A1-2A9872AF9F2D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1963,19 +1939,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1694.683</c:v>
+                  <c:v>1687.7760000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3054.7429999999999</c:v>
+                  <c:v>3038.3829999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4564.6719999999996</c:v>
+                  <c:v>4544.3850000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6169.3270000000002</c:v>
+                  <c:v>6168.4139999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7782.5370000000003</c:v>
+                  <c:v>7814.0439999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1987,13 +1963,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.94199999999999995</c:v>
+                  <c:v>0.94299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.95499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.96</c:v>
+                  <c:v>0.96099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.96399999999999997</c:v>
@@ -2007,7 +1983,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-93CF-42C8-8040-8C395A4F1355}"/>
+              <c16:uniqueId val="{00000001-C495-48D9-A0A1-2A9872AF9F2D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2195,7 +2171,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-82D9-439B-AABB-5369EC2C4F53}"/>
+              <c16:uniqueId val="{00000000-858C-4415-A6E3-2FFD1748E910}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2224,19 +2200,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1958.4349999999999</c:v>
+                  <c:v>1955.704</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3420.1039999999998</c:v>
+                  <c:v>3387.0590000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4916.0770000000002</c:v>
+                  <c:v>4960.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6403.6580000000004</c:v>
+                  <c:v>6385.7460000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7897.9560000000001</c:v>
+                  <c:v>7891.9380000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2248,19 +2224,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.950000000000003</c:v>
+                  <c:v>37.043999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.563000000000002</c:v>
+                  <c:v>38.597999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.604999999999997</c:v>
+                  <c:v>39.665999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.319000000000003</c:v>
+                  <c:v>40.334000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.838999999999999</c:v>
+                  <c:v>40.857999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2268,7 +2244,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-82D9-439B-AABB-5369EC2C4F53}"/>
+              <c16:uniqueId val="{00000001-858C-4415-A6E3-2FFD1748E910}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2457,7 +2433,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0654-4AE3-8807-3872953E05DE}"/>
+              <c16:uniqueId val="{00000000-5582-49BE-B475-B26710A45603}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2486,19 +2462,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1958.4349999999999</c:v>
+                  <c:v>1955.704</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3420.1039999999998</c:v>
+                  <c:v>3387.0590000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4916.0770000000002</c:v>
+                  <c:v>4960.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6403.6580000000004</c:v>
+                  <c:v>6385.7460000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7897.9560000000001</c:v>
+                  <c:v>7891.9380000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2510,16 +2486,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.92300000000000004</c:v>
+                  <c:v>0.92500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94199999999999995</c:v>
+                  <c:v>0.94299999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.95199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.95699999999999996</c:v>
+                  <c:v>0.95799999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.96099999999999997</c:v>
@@ -2530,7 +2506,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0654-4AE3-8807-3872953E05DE}"/>
+              <c16:uniqueId val="{00000001-5582-49BE-B475-B26710A45603}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2718,7 +2694,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F5EC-4B4F-9BCD-059E4808EE2B}"/>
+              <c16:uniqueId val="{00000000-51CF-4F96-A7BC-3FB086B95A59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2731,7 +2707,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>testgPSNR</c:v>
+                  <c:v>xin266gPSNR</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2747,19 +2723,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2000.2470000000001</c:v>
+                  <c:v>1997.6679999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3508.6239999999998</c:v>
+                  <c:v>3506.7620000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5006.8100000000004</c:v>
+                  <c:v>5006.0969999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6524.6260000000002</c:v>
+                  <c:v>6538.5540000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8072.7349999999997</c:v>
+                  <c:v>8064.5529999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2771,19 +2747,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>37.526000000000003</c:v>
+                  <c:v>37.582000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.804000000000002</c:v>
+                  <c:v>38.829000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.429000000000002</c:v>
+                  <c:v>39.436999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.798999999999999</c:v>
+                  <c:v>39.808999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.067</c:v>
+                  <c:v>40.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2791,7 +2767,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F5EC-4B4F-9BCD-059E4808EE2B}"/>
+              <c16:uniqueId val="{00000001-51CF-4F96-A7BC-3FB086B95A59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2980,7 +2956,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-45BA-4622-901B-845AD8A7F012}"/>
+              <c16:uniqueId val="{00000000-1C2C-47D3-B613-67A86C3BD4F9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2993,7 +2969,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>testgSSIM</c:v>
+                  <c:v>xin266gSSIM</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3009,19 +2985,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2000.2470000000001</c:v>
+                  <c:v>1997.6679999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3508.6239999999998</c:v>
+                  <c:v>3506.7620000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5006.8100000000004</c:v>
+                  <c:v>5006.0969999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6524.6260000000002</c:v>
+                  <c:v>6538.5540000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8072.7349999999997</c:v>
+                  <c:v>8064.5529999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3053,7 +3029,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-45BA-4622-901B-845AD8A7F012}"/>
+              <c16:uniqueId val="{00000001-1C2C-47D3-B613-67A86C3BD4F9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3241,7 +3217,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EE92-41EB-8171-FA07E9E6B853}"/>
+              <c16:uniqueId val="{00000000-2BCD-4A14-A477-0E8699BDCF18}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3270,19 +3246,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1979.6859999999999</c:v>
+                  <c:v>1980.694</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3482.3560000000002</c:v>
+                  <c:v>3494.1410000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5147.6049999999996</c:v>
+                  <c:v>5124.3310000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6668.03</c:v>
+                  <c:v>6666.567</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8327.1810000000005</c:v>
+                  <c:v>8322.8310000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3294,16 +3270,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>36.274000000000001</c:v>
+                  <c:v>36.283000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.686999999999998</c:v>
+                  <c:v>36.691000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.956000000000003</c:v>
+                  <c:v>36.953000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.151000000000003</c:v>
+                  <c:v>37.152000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>37.319000000000003</c:v>
@@ -3314,7 +3290,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EE92-41EB-8171-FA07E9E6B853}"/>
+              <c16:uniqueId val="{00000001-2BCD-4A14-A477-0E8699BDCF18}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4199,9 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4210,19 +4184,19 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4233,19 +4207,19 @@
         <v>0.41</v>
       </c>
       <c r="C2">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
       <c r="D2">
-        <v>0.43</v>
+        <v>0.49</v>
       </c>
       <c r="E2">
-        <v>0.27</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F2">
         <v>0.31</v>
       </c>
       <c r="G2">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4253,22 +4227,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-19.59</v>
+        <v>-19.88</v>
       </c>
       <c r="C3">
-        <v>-16.91</v>
+        <v>-18.829999999999998</v>
       </c>
       <c r="D3">
-        <v>-13.45</v>
+        <v>-15.2</v>
       </c>
       <c r="E3">
-        <v>-12.94</v>
+        <v>-14.13</v>
       </c>
       <c r="F3">
-        <v>-30.84</v>
+        <v>-30.98</v>
       </c>
       <c r="G3">
-        <v>-22.89</v>
+        <v>-24.6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4279,19 +4253,19 @@
         <v>0.46</v>
       </c>
       <c r="C4">
-        <v>0.47</v>
+        <v>0.52</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E4">
-        <v>0.36</v>
+        <v>0.38</v>
       </c>
       <c r="F4">
         <v>0.33</v>
       </c>
       <c r="G4">
-        <v>0.46</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4299,22 +4273,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-22.05</v>
+        <v>-22.38</v>
       </c>
       <c r="C5">
-        <v>-18.739999999999998</v>
+        <v>-20.65</v>
       </c>
       <c r="D5">
-        <v>-16.02</v>
+        <v>-17.77</v>
       </c>
       <c r="E5">
-        <v>-16.899999999999999</v>
+        <v>-18.05</v>
       </c>
       <c r="F5">
-        <v>-32.159999999999997</v>
+        <v>-32.29</v>
       </c>
       <c r="G5">
-        <v>-26.07</v>
+        <v>-27.72</v>
       </c>
     </row>
   </sheetData>
@@ -4355,18 +4329,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1947.596</v>
@@ -4387,18 +4361,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>39.904000000000003</v>
@@ -4418,7 +4392,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>43.831000000000003</v>
@@ -4438,7 +4412,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>45.2</v>
@@ -4458,7 +4432,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.94799999999999995</v>
@@ -4478,7 +4452,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>40.963999999999999</v>
@@ -4498,7 +4472,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.95599999999999996</v>
@@ -4518,33 +4492,33 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1979.5830000000001</v>
+        <v>1979.192</v>
       </c>
       <c r="C11">
-        <v>3468.1219999999998</v>
+        <v>3459.5880000000002</v>
       </c>
       <c r="D11">
-        <v>4949.857</v>
+        <v>4951.4560000000001</v>
       </c>
       <c r="E11">
-        <v>6437.558</v>
+        <v>6478.2920000000004</v>
       </c>
       <c r="F11">
-        <v>7995.3590000000004</v>
+        <v>7993.6930000000002</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>40.655999999999999</v>
+        <v>40.664000000000001</v>
       </c>
       <c r="C12">
-        <v>41.877000000000002</v>
+        <v>41.878</v>
       </c>
       <c r="D12">
         <v>42.414999999999999</v>
@@ -4553,52 +4527,52 @@
         <v>42.719000000000001</v>
       </c>
       <c r="F12">
-        <v>42.935000000000002</v>
+        <v>42.933999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>45.021999999999998</v>
+        <v>45.037999999999997</v>
       </c>
       <c r="C13">
-        <v>45.996000000000002</v>
+        <v>46.003</v>
       </c>
       <c r="D13">
-        <v>46.436999999999998</v>
+        <v>46.441000000000003</v>
       </c>
       <c r="E13">
-        <v>46.707999999999998</v>
+        <v>46.709000000000003</v>
       </c>
       <c r="F13">
-        <v>46.915999999999997</v>
+        <v>46.914999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>46.503</v>
+        <v>46.515999999999998</v>
       </c>
       <c r="C14">
-        <v>47.665999999999997</v>
+        <v>47.667999999999999</v>
       </c>
       <c r="D14">
-        <v>48.165999999999997</v>
+        <v>48.17</v>
       </c>
       <c r="E14">
-        <v>48.487000000000002</v>
+        <v>48.488</v>
       </c>
       <c r="F14">
-        <v>48.718000000000004</v>
+        <v>48.719000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.95399999999999996</v>
@@ -4618,27 +4592,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>41.786000000000001</v>
+        <v>41.793999999999997</v>
       </c>
       <c r="C16">
-        <v>42.982999999999997</v>
+        <v>42.984999999999999</v>
       </c>
       <c r="D16">
-        <v>43.511000000000003</v>
+        <v>43.512</v>
       </c>
       <c r="E16">
         <v>43.813000000000002</v>
       </c>
       <c r="F16">
-        <v>44.029000000000003</v>
+        <v>44.027999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.96199999999999997</v>
@@ -4694,18 +4668,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1611.8019999999999</v>
@@ -4726,18 +4700,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>38.012999999999998</v>
@@ -4757,7 +4731,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>40.798000000000002</v>
@@ -4777,7 +4751,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>42.066000000000003</v>
@@ -4797,7 +4771,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.93</v>
@@ -4817,7 +4791,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>38.875</v>
@@ -4837,7 +4811,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.93500000000000005</v>
@@ -4857,90 +4831,90 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1694.683</v>
+        <v>1687.7760000000001</v>
       </c>
       <c r="C11">
-        <v>3054.7429999999999</v>
+        <v>3038.3829999999998</v>
       </c>
       <c r="D11">
-        <v>4564.6719999999996</v>
+        <v>4544.3850000000002</v>
       </c>
       <c r="E11">
-        <v>6169.3270000000002</v>
+        <v>6168.4139999999998</v>
       </c>
       <c r="F11">
-        <v>7782.5370000000003</v>
+        <v>7814.0439999999999</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>38.765999999999998</v>
+        <v>38.862000000000002</v>
       </c>
       <c r="C12">
-        <v>40.424999999999997</v>
+        <v>40.468000000000004</v>
       </c>
       <c r="D12">
-        <v>41.289000000000001</v>
+        <v>41.31</v>
       </c>
       <c r="E12">
-        <v>41.801000000000002</v>
+        <v>41.819000000000003</v>
       </c>
       <c r="F12">
-        <v>42.134999999999998</v>
+        <v>42.148000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>41.716999999999999</v>
+        <v>41.777000000000001</v>
       </c>
       <c r="C13">
-        <v>42.758000000000003</v>
+        <v>42.796999999999997</v>
       </c>
       <c r="D13">
-        <v>43.383000000000003</v>
+        <v>43.402999999999999</v>
       </c>
       <c r="E13">
-        <v>43.790999999999997</v>
+        <v>43.811</v>
       </c>
       <c r="F13">
-        <v>44.1</v>
+        <v>44.115000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>42.765999999999998</v>
+        <v>42.832999999999998</v>
       </c>
       <c r="C14">
-        <v>44.088000000000001</v>
+        <v>44.125</v>
       </c>
       <c r="D14">
-        <v>44.957000000000001</v>
+        <v>44.982999999999997</v>
       </c>
       <c r="E14">
-        <v>45.595999999999997</v>
+        <v>45.628</v>
       </c>
       <c r="F14">
-        <v>46.058999999999997</v>
+        <v>46.091999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>0.93700000000000006</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="C15">
         <v>0.95199999999999996</v>
@@ -4957,36 +4931,36 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>39.640999999999998</v>
+        <v>39.731000000000002</v>
       </c>
       <c r="C16">
-        <v>41.204000000000001</v>
+        <v>41.246000000000002</v>
       </c>
       <c r="D16">
-        <v>42.04</v>
+        <v>42.061</v>
       </c>
       <c r="E16">
-        <v>42.55</v>
+        <v>42.569000000000003</v>
       </c>
       <c r="F16">
-        <v>42.890999999999998</v>
+        <v>42.905999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>0.94199999999999995</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="C17">
         <v>0.95499999999999996</v>
       </c>
       <c r="D17">
-        <v>0.96</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="E17">
         <v>0.96399999999999997</v>
@@ -5033,18 +5007,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1834.664</v>
@@ -5065,18 +5039,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>35.253</v>
@@ -5096,7 +5070,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>38.774000000000001</v>
@@ -5116,7 +5090,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>39.911999999999999</v>
@@ -5136,7 +5110,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.90600000000000003</v>
@@ -5156,7 +5130,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>36.234000000000002</v>
@@ -5176,7 +5150,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.91</v>
@@ -5196,96 +5170,96 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1958.4349999999999</v>
+        <v>1955.704</v>
       </c>
       <c r="C11">
-        <v>3420.1039999999998</v>
+        <v>3387.0590000000002</v>
       </c>
       <c r="D11">
-        <v>4916.0770000000002</v>
+        <v>4960.25</v>
       </c>
       <c r="E11">
-        <v>6403.6580000000004</v>
+        <v>6385.7460000000001</v>
       </c>
       <c r="F11">
-        <v>7897.9560000000001</v>
+        <v>7891.9380000000001</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>35.887</v>
+        <v>35.984000000000002</v>
       </c>
       <c r="C12">
-        <v>37.6</v>
+        <v>37.634999999999998</v>
       </c>
       <c r="D12">
-        <v>38.691000000000003</v>
+        <v>38.752000000000002</v>
       </c>
       <c r="E12">
-        <v>39.433</v>
+        <v>39.445999999999998</v>
       </c>
       <c r="F12">
-        <v>39.973999999999997</v>
+        <v>39.991</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>40.061</v>
+        <v>40.131999999999998</v>
       </c>
       <c r="C13">
-        <v>41.116999999999997</v>
+        <v>41.146000000000001</v>
       </c>
       <c r="D13">
-        <v>41.847000000000001</v>
+        <v>41.893000000000001</v>
       </c>
       <c r="E13">
-        <v>42.353000000000002</v>
+        <v>42.368000000000002</v>
       </c>
       <c r="F13">
-        <v>42.713999999999999</v>
+        <v>42.73</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>40.908000000000001</v>
+        <v>40.981999999999999</v>
       </c>
       <c r="C14">
-        <v>42.01</v>
+        <v>42.057000000000002</v>
       </c>
       <c r="D14">
-        <v>42.918999999999997</v>
+        <v>42.991</v>
       </c>
       <c r="E14">
-        <v>43.610999999999997</v>
+        <v>43.646999999999998</v>
       </c>
       <c r="F14">
-        <v>44.133000000000003</v>
+        <v>44.164000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>0.91700000000000004</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="C15">
         <v>0.93899999999999995</v>
       </c>
       <c r="D15">
-        <v>0.94899999999999995</v>
+        <v>0.95</v>
       </c>
       <c r="E15">
         <v>0.95499999999999996</v>
@@ -5296,39 +5270,39 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>36.950000000000003</v>
+        <v>37.043999999999997</v>
       </c>
       <c r="C16">
-        <v>38.563000000000002</v>
+        <v>38.597999999999999</v>
       </c>
       <c r="D16">
-        <v>39.604999999999997</v>
+        <v>39.665999999999997</v>
       </c>
       <c r="E16">
-        <v>40.319000000000003</v>
+        <v>40.334000000000003</v>
       </c>
       <c r="F16">
-        <v>40.838999999999999</v>
+        <v>40.857999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>0.92300000000000004</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="C17">
-        <v>0.94199999999999995</v>
+        <v>0.94299999999999995</v>
       </c>
       <c r="D17">
         <v>0.95199999999999996</v>
       </c>
       <c r="E17">
-        <v>0.95699999999999996</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="F17">
         <v>0.96099999999999997</v>
@@ -5372,18 +5346,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>2012.836</v>
@@ -5404,18 +5378,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>35.896000000000001</v>
@@ -5435,7 +5409,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>40.999000000000002</v>
@@ -5455,7 +5429,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>40.970999999999997</v>
@@ -5475,7 +5449,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5495,7 +5469,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>37.030999999999999</v>
@@ -5515,7 +5489,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.91300000000000003</v>
@@ -5535,90 +5509,90 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>2000.2470000000001</v>
+        <v>1997.6679999999999</v>
       </c>
       <c r="C11">
-        <v>3508.6239999999998</v>
+        <v>3506.7620000000002</v>
       </c>
       <c r="D11">
-        <v>5006.8100000000004</v>
+        <v>5006.0969999999998</v>
       </c>
       <c r="E11">
-        <v>6524.6260000000002</v>
+        <v>6538.5540000000001</v>
       </c>
       <c r="F11">
-        <v>8072.7349999999997</v>
+        <v>8064.5529999999999</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>36.29</v>
+        <v>36.347999999999999</v>
       </c>
       <c r="C12">
-        <v>37.576000000000001</v>
+        <v>37.601999999999997</v>
       </c>
       <c r="D12">
-        <v>38.207999999999998</v>
+        <v>38.216000000000001</v>
       </c>
       <c r="E12">
-        <v>38.585000000000001</v>
+        <v>38.594000000000001</v>
       </c>
       <c r="F12">
-        <v>38.86</v>
+        <v>38.862000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>42.027999999999999</v>
+        <v>42.070999999999998</v>
       </c>
       <c r="C13">
-        <v>43.006</v>
+        <v>43.027999999999999</v>
       </c>
       <c r="D13">
-        <v>43.463999999999999</v>
+        <v>43.472000000000001</v>
       </c>
       <c r="E13">
-        <v>43.715000000000003</v>
+        <v>43.723999999999997</v>
       </c>
       <c r="F13">
-        <v>43.887</v>
+        <v>43.893000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>42.35</v>
+        <v>42.402999999999999</v>
       </c>
       <c r="C14">
-        <v>43.838000000000001</v>
+        <v>43.871000000000002</v>
       </c>
       <c r="D14">
-        <v>44.564</v>
+        <v>44.576999999999998</v>
       </c>
       <c r="E14">
-        <v>44.970999999999997</v>
+        <v>44.984999999999999</v>
       </c>
       <c r="F14">
-        <v>45.25</v>
+        <v>45.256999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>0.9</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="C15">
         <v>0.91700000000000004</v>
@@ -5627,7 +5601,7 @@
         <v>0.92400000000000004</v>
       </c>
       <c r="E15">
-        <v>0.92800000000000005</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="F15">
         <v>0.93200000000000005</v>
@@ -5635,27 +5609,27 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>37.526000000000003</v>
+        <v>37.582000000000001</v>
       </c>
       <c r="C16">
-        <v>38.804000000000002</v>
+        <v>38.829000000000001</v>
       </c>
       <c r="D16">
-        <v>39.429000000000002</v>
+        <v>39.436999999999998</v>
       </c>
       <c r="E16">
-        <v>39.798999999999999</v>
+        <v>39.808999999999997</v>
       </c>
       <c r="F16">
-        <v>40.067</v>
+        <v>40.07</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.92100000000000004</v>
@@ -5684,9 +5658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -5713,18 +5685,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1984.951</v>
@@ -5745,18 +5717,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>34.497</v>
@@ -5776,7 +5748,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>40.106999999999999</v>
@@ -5796,7 +5768,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>42.6</v>
@@ -5816,7 +5788,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.89300000000000002</v>
@@ -5836,7 +5808,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>35.814999999999998</v>
@@ -5856,7 +5828,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.90900000000000003</v>
@@ -5876,39 +5848,39 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1979.6859999999999</v>
+        <v>1980.694</v>
       </c>
       <c r="C11">
-        <v>3482.3560000000002</v>
+        <v>3494.1410000000001</v>
       </c>
       <c r="D11">
-        <v>5147.6049999999996</v>
+        <v>5124.3310000000001</v>
       </c>
       <c r="E11">
-        <v>6668.03</v>
+        <v>6666.567</v>
       </c>
       <c r="F11">
-        <v>8327.1810000000005</v>
+        <v>8322.8310000000001</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>34.918999999999997</v>
+        <v>34.927</v>
       </c>
       <c r="C12">
-        <v>35.341000000000001</v>
+        <v>35.344999999999999</v>
       </c>
       <c r="D12">
-        <v>35.610999999999997</v>
+        <v>35.607999999999997</v>
       </c>
       <c r="E12">
-        <v>35.804000000000002</v>
+        <v>35.805</v>
       </c>
       <c r="F12">
         <v>35.975000000000001</v>
@@ -5916,47 +5888,47 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>41.023000000000003</v>
+        <v>41.039000000000001</v>
       </c>
       <c r="C13">
-        <v>41.363</v>
+        <v>41.362000000000002</v>
       </c>
       <c r="D13">
-        <v>41.631999999999998</v>
+        <v>41.636000000000003</v>
       </c>
       <c r="E13">
-        <v>41.845999999999997</v>
+        <v>41.850999999999999</v>
       </c>
       <c r="F13">
-        <v>41.994</v>
+        <v>41.991</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>43.259</v>
+        <v>43.279000000000003</v>
       </c>
       <c r="C14">
-        <v>43.546999999999997</v>
+        <v>43.558999999999997</v>
       </c>
       <c r="D14">
-        <v>43.792999999999999</v>
+        <v>43.793999999999997</v>
       </c>
       <c r="E14">
-        <v>43.993000000000002</v>
+        <v>43.991999999999997</v>
       </c>
       <c r="F14">
-        <v>44.145000000000003</v>
+        <v>44.134999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>0.9</v>
@@ -5976,19 +5948,19 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>36.274000000000001</v>
+        <v>36.283000000000001</v>
       </c>
       <c r="C16">
-        <v>36.686999999999998</v>
+        <v>36.691000000000003</v>
       </c>
       <c r="D16">
-        <v>36.956000000000003</v>
+        <v>36.953000000000003</v>
       </c>
       <c r="E16">
-        <v>37.151000000000003</v>
+        <v>37.152000000000001</v>
       </c>
       <c r="F16">
         <v>37.319000000000003</v>
@@ -5996,7 +5968,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>0.91600000000000004</v>
@@ -6052,18 +6024,18 @@
         <v>0</v>
       </c>
       <c r="R1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>1960.646</v>
@@ -6084,18 +6056,18 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3">
         <v>35.564999999999998</v>
@@ -6115,7 +6087,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>38.436</v>
@@ -6135,7 +6107,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>40.572000000000003</v>
@@ -6155,7 +6127,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>0.9</v>
@@ -6175,7 +6147,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>36.505000000000003</v>
@@ -6195,7 +6167,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8">
         <v>0.90700000000000003</v>
@@ -6215,90 +6187,90 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B11">
-        <v>1986.807</v>
+        <v>1991.7719999999999</v>
       </c>
       <c r="C11">
-        <v>3473.232</v>
+        <v>3466.739</v>
       </c>
       <c r="D11">
-        <v>4952.0559999999996</v>
+        <v>4937.6760000000004</v>
       </c>
       <c r="E11">
-        <v>6456.8239999999996</v>
+        <v>6456.4110000000001</v>
       </c>
       <c r="F11">
-        <v>7943.57</v>
+        <v>7928.8059999999996</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>36.143000000000001</v>
+        <v>36.225999999999999</v>
       </c>
       <c r="C12">
-        <v>37.267000000000003</v>
+        <v>37.290999999999997</v>
       </c>
       <c r="D12">
-        <v>37.759</v>
+        <v>37.771999999999998</v>
       </c>
       <c r="E12">
-        <v>38.042000000000002</v>
+        <v>38.048000000000002</v>
       </c>
       <c r="F12">
-        <v>38.228000000000002</v>
+        <v>38.234999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B13">
-        <v>39.116</v>
+        <v>39.158999999999999</v>
       </c>
       <c r="C13">
-        <v>39.591999999999999</v>
+        <v>39.61</v>
       </c>
       <c r="D13">
-        <v>39.844999999999999</v>
+        <v>39.856000000000002</v>
       </c>
       <c r="E13">
-        <v>40.024999999999999</v>
+        <v>40.034999999999997</v>
       </c>
       <c r="F13">
-        <v>40.170999999999999</v>
+        <v>40.176000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>41.749000000000002</v>
+        <v>41.835999999999999</v>
       </c>
       <c r="C14">
-        <v>42.691000000000003</v>
+        <v>42.713000000000001</v>
       </c>
       <c r="D14">
-        <v>43.192999999999998</v>
+        <v>43.212000000000003</v>
       </c>
       <c r="E14">
-        <v>43.529000000000003</v>
+        <v>43.548999999999999</v>
       </c>
       <c r="F14">
-        <v>43.771000000000001</v>
+        <v>43.78</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15">
-        <v>0.90800000000000003</v>
+        <v>0.91</v>
       </c>
       <c r="C15">
         <v>0.92200000000000004</v>
@@ -6315,30 +6287,30 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>37.131</v>
+        <v>37.21</v>
       </c>
       <c r="C16">
-        <v>38.170999999999999</v>
+        <v>38.194000000000003</v>
       </c>
       <c r="D16">
-        <v>38.634</v>
+        <v>38.646999999999998</v>
       </c>
       <c r="E16">
-        <v>38.906999999999996</v>
+        <v>38.914000000000001</v>
       </c>
       <c r="F16">
-        <v>39.091999999999999</v>
+        <v>39.097999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B17">
-        <v>0.91700000000000004</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="C17">
         <v>0.92800000000000005</v>

</xml_diff>